<commit_message>
Started adding Logging of methods
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/Bball SQL.xlsx
+++ b/BballMVC/_Documentation/Bball SQL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A93F051-76A5-4FDB-9250-E339910068F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D90F32C-2DEF-48C5-BF3D-982C5947E630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59190" yWindow="765" windowWidth="22350" windowHeight="13470" tabRatio="831" activeTab="6" xr2:uid="{3CF9E211-50E1-4178-837C-51B36022A708}"/>
+    <workbookView xWindow="765" yWindow="825" windowWidth="27045" windowHeight="14280" tabRatio="831" activeTab="5" xr2:uid="{3CF9E211-50E1-4178-837C-51B36022A708}"/>
   </bookViews>
   <sheets>
     <sheet name="SPs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'Migrate DB'!$A$1:$E$95</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">uspCalcTodaysMatchups!$A$1:$I$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">uspCalcTodaysMatchups!$A$1:$I$71</definedName>
     <definedName name="TmTL">'Avg Atmp'!$A$2</definedName>
     <definedName name="TotAtmps">'Avg Atmp'!$E$3</definedName>
   </definedNames>
@@ -50,6 +50,47 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Keith</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{EE2F014B-DBE2-400B-A0C1-F919CB6A0134}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">StartDate: Add StartDate as well as GamesBack
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E44" authorId="0" shapeId="0" xr:uid="{E87E8845-7127-490F-A019-21205554E175}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">@varLgAvgGamesBack
+   Vary depending upon Lg Variance 
+  IE  play off
+ </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Keith</author>
@@ -78,7 +119,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Keith</author>
@@ -104,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="531">
   <si>
     <t>Name</t>
   </si>
@@ -2318,9 +2359,6 @@
     <t>Rot#/Gm Time</t>
   </si>
   <si>
-    <t>ToDo--&gt;</t>
-  </si>
-  <si>
     <t>Section</t>
   </si>
   <si>
@@ -2358,6 +2396,12 @@
   </si>
   <si>
     <t>Ver Year</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>VenueBoth</t>
   </si>
 </sst>
 </file>
@@ -2367,7 +2411,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2438,6 +2482,12 @@
       <sz val="11"/>
       <color rgb="FF005259"/>
       <name val="Titillium Web"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -2605,7 +2655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -2713,7 +2763,6 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2735,6 +2784,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2765,8 +2823,8 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>381649</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>514475</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133475</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2809,7 +2867,7 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>295912</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>95423</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3930,7 +3988,7 @@
       <c r="A1" t="s">
         <v>494</v>
       </c>
-      <c r="B1" s="51">
+      <c r="B1" s="50">
         <v>231</v>
       </c>
     </row>
@@ -3977,7 +4035,7 @@
       <c r="A6" t="s">
         <v>498</v>
       </c>
-      <c r="B6" s="51">
+      <c r="B6" s="50">
         <v>4</v>
       </c>
     </row>
@@ -3985,7 +4043,7 @@
       <c r="A7" t="s">
         <v>499</v>
       </c>
-      <c r="B7" s="51">
+      <c r="B7" s="50">
         <v>12</v>
       </c>
       <c r="D7" s="44"/>
@@ -4030,7 +4088,7 @@
         <f>B10*B8 + B2</f>
         <v>242.26145833333334</v>
       </c>
-      <c r="W11" s="52" t="s">
+      <c r="W11" s="51" t="s">
         <v>505</v>
       </c>
     </row>
@@ -4221,11 +4279,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="J1" s="56" t="s">
+      <c r="J1" s="55" t="s">
         <v>372</v>
       </c>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
@@ -4275,7 +4333,7 @@
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="55" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -4286,7 +4344,7 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="B4" s="56"/>
+      <c r="B4" s="55"/>
       <c r="C4" s="10" t="s">
         <v>378</v>
       </c>
@@ -4295,7 +4353,7 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="B5" s="56"/>
+      <c r="B5" s="55"/>
       <c r="C5" s="10" t="s">
         <v>379</v>
       </c>
@@ -6767,7 +6825,7 @@
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="28" spans="1:3" ht="11.25" customHeight="1">
-      <c r="A28" s="57" t="s">
+      <c r="A28" s="56" t="s">
         <v>69</v>
       </c>
       <c r="B28" s="19" t="s">
@@ -6778,7 +6836,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="12" customHeight="1">
-      <c r="A29" s="58"/>
+      <c r="A29" s="57"/>
       <c r="B29" s="20" t="s">
         <v>72</v>
       </c>
@@ -6787,14 +6845,14 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A30" s="58"/>
+      <c r="A30" s="57"/>
       <c r="B30" s="21"/>
       <c r="C30" s="24" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A31" s="59"/>
+      <c r="A31" s="58"/>
       <c r="B31" s="18"/>
       <c r="C31" s="17" t="s">
         <v>70</v>
@@ -7512,13 +7570,13 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0274D91-97AE-4EB7-A37C-618C93529D3A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0274D91-97AE-4EB7-A37C-618C93529D3A}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V75"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7535,41 +7593,41 @@
     <col min="22" max="22" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
-      <c r="A1" s="27" t="s">
-        <v>517</v>
-      </c>
-      <c r="B1" s="27" t="s">
+    <row r="1" spans="1:22" s="61" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A1" s="59" t="s">
+        <v>516</v>
+      </c>
+      <c r="B1" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="59" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="59" t="s">
         <v>230</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="59" t="s">
         <v>448</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="59" t="s">
         <v>454</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="59" t="s">
         <v>347</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="60" t="s">
         <v>348</v>
       </c>
-      <c r="I1" t="str">
+      <c r="I1" s="61" t="str">
         <f>"SELECT  max(GameDate) as " &amp; D1 &amp; "MaxDate FROM " &amp; D1</f>
         <v>SELECT  max(GameDate) as Table OutMaxDate FROM Table Out</v>
       </c>
     </row>
     <row r="2" spans="1:22">
-      <c r="A2" s="53">
+      <c r="A2" s="52">
         <v>1</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="52" t="s">
         <v>208</v>
       </c>
     </row>
@@ -7631,7 +7689,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="9" spans="1:22" hidden="1">
+    <row r="9" spans="1:22">
       <c r="B9" t="s">
         <v>187</v>
       </c>
@@ -7642,7 +7700,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:22" hidden="1">
+    <row r="10" spans="1:22">
       <c r="B10" t="s">
         <v>188</v>
       </c>
@@ -7653,7 +7711,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="11" spans="1:22" hidden="1">
+    <row r="11" spans="1:22">
       <c r="B11" t="s">
         <v>189</v>
       </c>
@@ -7667,7 +7725,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:22" hidden="1">
+    <row r="12" spans="1:22">
       <c r="B12" t="s">
         <v>190</v>
       </c>
@@ -7675,40 +7733,40 @@
         <v>249</v>
       </c>
     </row>
-    <row r="13" spans="1:22" hidden="1">
+    <row r="13" spans="1:22">
       <c r="B13" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="14" spans="1:22" hidden="1">
+    <row r="14" spans="1:22">
       <c r="B14" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="15" spans="1:22" hidden="1">
+    <row r="15" spans="1:22">
       <c r="B15" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="30" hidden="1">
+    <row r="16" spans="1:22" ht="30">
       <c r="B16" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:11" hidden="1">
+    <row r="17" spans="1:11">
       <c r="B17" s="3" t="s">
         <v>241</v>
       </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:11" hidden="1">
+    <row r="18" spans="1:11">
       <c r="B18" s="3" t="s">
         <v>491</v>
       </c>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:11" hidden="1">
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>1.41</v>
       </c>
@@ -7716,11 +7774,14 @@
         <v>492</v>
       </c>
       <c r="C19" s="3"/>
+      <c r="E19" t="s">
+        <v>454</v>
+      </c>
       <c r="F19" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1">
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>1.5</v>
       </c>
@@ -7731,19 +7792,19 @@
         <v>232</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1">
+    <row r="21" spans="1:11">
       <c r="B21" s="3" t="s">
         <v>193</v>
       </c>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:11" hidden="1">
+    <row r="22" spans="1:11">
       <c r="B22" s="3" t="s">
         <v>194</v>
       </c>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:11" hidden="1">
+    <row r="23" spans="1:11">
       <c r="A23">
         <v>1.6</v>
       </c>
@@ -7751,7 +7812,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1">
+    <row r="24" spans="1:11">
       <c r="B24" s="30" t="s">
         <v>360</v>
       </c>
@@ -7759,7 +7820,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1">
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>1.7</v>
       </c>
@@ -7771,7 +7832,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1">
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>1.8</v>
       </c>
@@ -7788,7 +7849,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1">
+    <row r="27" spans="1:11">
       <c r="A27">
         <v>1.9</v>
       </c>
@@ -7806,7 +7867,7 @@
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
     </row>
-    <row r="28" spans="1:11" hidden="1">
+    <row r="28" spans="1:11">
       <c r="B28" s="2" t="s">
         <v>199</v>
       </c>
@@ -7814,14 +7875,16 @@
       <c r="D28" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="E28" s="13"/>
+      <c r="E28" s="13" t="s">
+        <v>454</v>
+      </c>
       <c r="F28" s="13" t="s">
         <v>201</v>
       </c>
       <c r="G28" s="13"/>
-      <c r="H28" s="50"/>
-    </row>
-    <row r="29" spans="1:11" hidden="1">
+      <c r="H28" s="49"/>
+    </row>
+    <row r="29" spans="1:11">
       <c r="B29" s="2" t="s">
         <v>202</v>
       </c>
@@ -7830,30 +7893,36 @@
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
-      <c r="H29" s="50"/>
+      <c r="H29" s="49"/>
       <c r="K29" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1">
+    <row r="30" spans="1:11">
       <c r="B30" s="30" t="s">
         <v>203</v>
       </c>
       <c r="C30" s="30"/>
+      <c r="E30" t="s">
+        <v>454</v>
+      </c>
       <c r="F30" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1">
+    <row r="31" spans="1:11">
       <c r="B31" s="30" t="s">
         <v>207</v>
       </c>
       <c r="C31" s="30"/>
+      <c r="E31" t="s">
+        <v>454</v>
+      </c>
       <c r="F31" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1">
+    <row r="32" spans="1:11">
       <c r="A32" s="31">
         <v>1.1000000000000001</v>
       </c>
@@ -7883,6 +7952,9 @@
       <c r="B35" s="6" t="s">
         <v>346</v>
       </c>
+      <c r="E35" t="s">
+        <v>454</v>
+      </c>
       <c r="F35" t="s">
         <v>490</v>
       </c>
@@ -7901,7 +7973,9 @@
       <c r="D36" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E36" s="14"/>
+      <c r="E36" t="s">
+        <v>529</v>
+      </c>
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -7914,6 +7988,9 @@
       <c r="D37" t="s">
         <v>186</v>
       </c>
+      <c r="E37" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="38" spans="1:8">
       <c r="B38" s="2" t="s">
@@ -7922,15 +7999,18 @@
       <c r="C38" t="s">
         <v>186</v>
       </c>
+      <c r="E38" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="53">
+      <c r="A39" s="52">
         <v>2</v>
       </c>
-      <c r="B39" s="54"/>
+      <c r="B39" s="53"/>
       <c r="C39" s="2"/>
       <c r="E39" t="s">
-        <v>516</v>
+        <v>359</v>
       </c>
       <c r="F39" t="s">
         <v>493</v>
@@ -7986,12 +8066,18 @@
       <c r="D44" t="s">
         <v>46</v>
       </c>
+      <c r="E44" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="45" spans="1:8">
       <c r="B45" s="5" t="s">
         <v>213</v>
       </c>
       <c r="C45" s="5"/>
+      <c r="E45" t="s">
+        <v>530</v>
+      </c>
     </row>
     <row r="46" spans="1:8">
       <c r="B46" s="5" t="s">
@@ -8000,10 +8086,10 @@
       <c r="C46" s="5"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="53">
+      <c r="A47" s="52">
         <v>3</v>
       </c>
-      <c r="B47" s="55" t="s">
+      <c r="B47" s="54" t="s">
         <v>215</v>
       </c>
       <c r="C47" s="32"/>
@@ -8103,10 +8189,10 @@
       <c r="C58" s="35"/>
     </row>
     <row r="59" spans="1:11">
-      <c r="A59" s="53">
+      <c r="A59" s="52">
         <v>4</v>
       </c>
-      <c r="B59" s="55" t="s">
+      <c r="B59" s="54" t="s">
         <v>236</v>
       </c>
     </row>
@@ -8251,10 +8337,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I38" xr:uid="{A7814D99-45DC-4222-B9C2-8A06FBE29E7B}"/>
+  <autoFilter ref="A1:I71" xr:uid="{A7814D99-45DC-4222-B9C2-8A06FBE29E7B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -8262,7 +8349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65609CE-B781-4EAF-B192-7D5E63B245CA}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -8277,70 +8364,70 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="47" t="s">
+        <v>522</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>521</v>
+      </c>
+      <c r="C1" s="47" t="s">
         <v>523</v>
       </c>
-      <c r="B1" s="47" t="s">
-        <v>522</v>
-      </c>
-      <c r="C1" s="47" t="s">
+      <c r="D1" s="47" t="s">
+        <v>528</v>
+      </c>
+      <c r="E1" s="47" t="s">
         <v>524</v>
-      </c>
-      <c r="D1" s="47" t="s">
-        <v>529</v>
-      </c>
-      <c r="E1" s="47" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>517</v>
+      </c>
+      <c r="B2" t="s">
         <v>518</v>
       </c>
-      <c r="B2" t="s">
-        <v>519</v>
-      </c>
       <c r="C2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D2">
         <v>2012</v>
       </c>
       <c r="E2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D3">
         <v>2017</v>
       </c>
       <c r="E3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D4">
         <v>2017</v>
       </c>
       <c r="E4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Branch 11 - Final on 02/11/2021
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/Bball SQL.xlsx
+++ b/BballMVC/_Documentation/Bball SQL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCB0E5B-FD61-4064-8B5F-0F0B269088AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8078A1B9-4012-408B-9CC5-EDBF12595E8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="3270" windowWidth="22815" windowHeight="14595" tabRatio="831" firstSheet="4" activeTab="13" xr2:uid="{3CF9E211-50E1-4178-837C-51B36022A708}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="25290" windowHeight="11835" tabRatio="831" firstSheet="14" activeTab="22" xr2:uid="{3CF9E211-50E1-4178-837C-51B36022A708}"/>
   </bookViews>
   <sheets>
     <sheet name="SPs" sheetId="1" r:id="rId1"/>
@@ -198,7 +198,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="654">
   <si>
     <t>Name</t>
   </si>
@@ -2913,6 +2913,9 @@
   </si>
   <si>
     <t>Single Line</t>
+  </si>
+  <si>
+    <t>BBALLHISTORY</t>
   </si>
 </sst>
 </file>
@@ -4565,10 +4568,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65609CE-B781-4EAF-B192-7D5E63B245CA}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4645,6 +4648,23 @@
         <v>2017</v>
       </c>
       <c r="E4" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>512</v>
+      </c>
+      <c r="B5" t="s">
+        <v>653</v>
+      </c>
+      <c r="C5" t="s">
+        <v>522</v>
+      </c>
+      <c r="D5">
+        <v>2017</v>
+      </c>
+      <c r="E5" t="s">
         <v>521</v>
       </c>
     </row>
@@ -5164,7 +5184,7 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
@@ -5970,7 +5990,7 @@
   <dimension ref="A1:E95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -8151,7 +8171,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A3:I44"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
@@ -8993,8 +9013,8 @@
   <dimension ref="A1:V116"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10584,7 +10604,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Added Bball Mgmt, Alert Err Msg to modal, added styles, "Canceled" msg on TMs UI, added "Loading" icon
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/Bball SQL.xlsx
+++ b/BballMVC/_Documentation/Bball SQL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8078A1B9-4012-408B-9CC5-EDBF12595E8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7550DE-78E5-4E2C-8402-50818974F00B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="25290" windowHeight="11835" tabRatio="831" firstSheet="14" activeTab="22" xr2:uid="{3CF9E211-50E1-4178-837C-51B36022A708}"/>
+    <workbookView xWindow="1425" yWindow="1050" windowWidth="26940" windowHeight="11835" tabRatio="831" firstSheet="3" activeTab="12" xr2:uid="{3CF9E211-50E1-4178-837C-51B36022A708}"/>
   </bookViews>
   <sheets>
     <sheet name="SPs" sheetId="1" r:id="rId1"/>
@@ -23,22 +23,21 @@
     <sheet name="LeagueInfo Rows" sheetId="21" r:id="rId8"/>
     <sheet name="Templates" sheetId="4" r:id="rId9"/>
     <sheet name="Instances" sheetId="20" r:id="rId10"/>
-    <sheet name="Bills ADJs" sheetId="18" r:id="rId11"/>
-    <sheet name="BSS Flow" sheetId="16" r:id="rId12"/>
-    <sheet name="CalcProjectedPoints" sheetId="12" r:id="rId13"/>
-    <sheet name="GameStatus" sheetId="19" r:id="rId14"/>
-    <sheet name="Avg Atmp" sheetId="14" r:id="rId15"/>
-    <sheet name="Post Gm" sheetId="13" r:id="rId16"/>
-    <sheet name="Migrate DB" sheetId="11" r:id="rId17"/>
-    <sheet name="Prod Tables to Delete" sheetId="23" r:id="rId18"/>
-    <sheet name="OurTotalLine Calculations" sheetId="8" r:id="rId19"/>
-    <sheet name="BSS Update process" sheetId="17" r:id="rId20"/>
-    <sheet name="Last Season History Screenshot" sheetId="5" r:id="rId21"/>
-    <sheet name="BoxScore Columns" sheetId="15" r:id="rId22"/>
-    <sheet name="Bball Screenshot" sheetId="7" r:id="rId23"/>
+    <sheet name="BSS Flow" sheetId="16" r:id="rId11"/>
+    <sheet name="CalcProjectedPoints" sheetId="12" r:id="rId12"/>
+    <sheet name="GameStatus" sheetId="19" r:id="rId13"/>
+    <sheet name="Avg Atmp" sheetId="14" r:id="rId14"/>
+    <sheet name="Post Gm" sheetId="13" r:id="rId15"/>
+    <sheet name="Migrate DB" sheetId="11" r:id="rId16"/>
+    <sheet name="Prod Tables to Delete" sheetId="23" r:id="rId17"/>
+    <sheet name="OurTotalLine Calculations" sheetId="8" r:id="rId18"/>
+    <sheet name="BSS Update process" sheetId="17" r:id="rId19"/>
+    <sheet name="Last Season History Screenshot" sheetId="5" r:id="rId20"/>
+    <sheet name="BoxScore Columns" sheetId="15" r:id="rId21"/>
+    <sheet name="Bball Screenshot" sheetId="7" r:id="rId22"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'Migrate DB'!$A$1:$E$95</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">'Migrate DB'!$A$1:$E$95</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">uspCalcTodaysMatchups!$A$1:$I$112</definedName>
     <definedName name="BxScLinePct">'Curve %'!$C$2</definedName>
     <definedName name="BxScTmStrPct">'Curve %'!$D$2</definedName>
@@ -198,7 +197,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="641">
   <si>
     <t>Name</t>
   </si>
@@ -2244,45 +2243,6 @@
   </si>
   <si>
     <t>Teams</t>
-  </si>
-  <si>
-    <t>Def</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATL                           </t>
-  </si>
-  <si>
-    <t>CHI</t>
-  </si>
-  <si>
-    <t>CON</t>
-  </si>
-  <si>
-    <t>DAL</t>
-  </si>
-  <si>
-    <t>IND</t>
-  </si>
-  <si>
-    <t>LAS</t>
-  </si>
-  <si>
-    <t>MIN</t>
-  </si>
-  <si>
-    <t>NYL</t>
-  </si>
-  <si>
-    <t>PHO</t>
-  </si>
-  <si>
-    <t>LVA</t>
-  </si>
-  <si>
-    <t>SEA</t>
-  </si>
-  <si>
-    <t>WAS</t>
   </si>
   <si>
     <t>Check Rotation for Games - Return If None</t>
@@ -3340,7 +3300,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -3446,7 +3406,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4585,87 +4544,87 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="46" t="s">
-        <v>517</v>
+        <v>504</v>
       </c>
       <c r="B1" s="46" t="s">
-        <v>516</v>
+        <v>503</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>518</v>
+        <v>505</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>523</v>
+        <v>510</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>519</v>
+        <v>506</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>512</v>
+        <v>499</v>
       </c>
       <c r="B2" t="s">
-        <v>513</v>
+        <v>500</v>
       </c>
       <c r="C2" t="s">
-        <v>520</v>
+        <v>507</v>
       </c>
       <c r="D2">
         <v>2012</v>
       </c>
       <c r="E2" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>512</v>
+        <v>499</v>
       </c>
       <c r="B3" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="C3" t="s">
-        <v>522</v>
+        <v>509</v>
       </c>
       <c r="D3">
         <v>2017</v>
       </c>
       <c r="E3" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>512</v>
+        <v>499</v>
       </c>
       <c r="B4" t="s">
-        <v>515</v>
+        <v>502</v>
       </c>
       <c r="C4" t="s">
-        <v>522</v>
+        <v>509</v>
       </c>
       <c r="D4">
         <v>2017</v>
       </c>
       <c r="E4" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>512</v>
+        <v>499</v>
       </c>
       <c r="B5" t="s">
-        <v>653</v>
+        <v>640</v>
       </c>
       <c r="C5" t="s">
-        <v>522</v>
+        <v>509</v>
       </c>
       <c r="D5">
         <v>2017</v>
       </c>
       <c r="E5" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
     </row>
   </sheetData>
@@ -4675,165 +4634,6 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2FCD9E5-810B-4ECB-B960-9878E4EA3925}">
-  <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="46" t="s">
-        <v>467</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>451</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="47" t="s">
-        <v>469</v>
-      </c>
-      <c r="B2" s="47">
-        <v>-3</v>
-      </c>
-      <c r="C2" s="47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="47" t="s">
-        <v>470</v>
-      </c>
-      <c r="B3" s="47">
-        <v>0</v>
-      </c>
-      <c r="C3" s="47">
-        <v>-1.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="47" t="s">
-        <v>471</v>
-      </c>
-      <c r="B4" s="47">
-        <v>0</v>
-      </c>
-      <c r="C4" s="47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="47" t="s">
-        <v>472</v>
-      </c>
-      <c r="B5" s="47">
-        <v>0</v>
-      </c>
-      <c r="C5" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="47" t="s">
-        <v>473</v>
-      </c>
-      <c r="B6" s="47">
-        <v>0</v>
-      </c>
-      <c r="C6" s="47">
-        <v>-1.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="47" t="s">
-        <v>474</v>
-      </c>
-      <c r="B7" s="47">
-        <v>0</v>
-      </c>
-      <c r="C7" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="47" t="s">
-        <v>475</v>
-      </c>
-      <c r="B8" s="47">
-        <v>0</v>
-      </c>
-      <c r="C8" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="47" t="s">
-        <v>476</v>
-      </c>
-      <c r="B9" s="47">
-        <v>-1</v>
-      </c>
-      <c r="C9" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="47" t="s">
-        <v>477</v>
-      </c>
-      <c r="B10" s="47">
-        <v>3</v>
-      </c>
-      <c r="C10" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="47" t="s">
-        <v>478</v>
-      </c>
-      <c r="B11" s="47">
-        <v>0</v>
-      </c>
-      <c r="C11" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="47" t="s">
-        <v>479</v>
-      </c>
-      <c r="B12" s="47">
-        <v>1</v>
-      </c>
-      <c r="C12" s="47">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="47" t="s">
-        <v>480</v>
-      </c>
-      <c r="B13" s="47">
-        <v>-3</v>
-      </c>
-      <c r="C13" s="47">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D318111E-043A-493E-A035-193861F809F6}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:I5"/>
@@ -4983,7 +4783,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8F1763-2684-48C3-A7E4-9194ED800D2A}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A3:M17"/>
@@ -5179,12 +4979,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80864BBB-D57C-4872-9528-539D35F75495}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
@@ -5196,7 +4996,7 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
-        <v>491</v>
+        <v>478</v>
       </c>
       <c r="B1" s="25">
         <v>2</v>
@@ -5204,7 +5004,7 @@
     </row>
     <row r="2" spans="1:23">
       <c r="A2" t="s">
-        <v>492</v>
+        <v>479</v>
       </c>
       <c r="B2" s="25">
         <v>0</v>
@@ -5212,7 +5012,7 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" t="s">
-        <v>493</v>
+        <v>480</v>
       </c>
       <c r="B3" s="25">
         <v>0</v>
@@ -5220,16 +5020,16 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>643</v>
-      </c>
-      <c r="B4" s="49">
+        <v>630</v>
+      </c>
+      <c r="B4" s="48">
         <f>gsMins*60 + csSecs</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:23">
       <c r="A5" t="s">
-        <v>641</v>
+        <v>628</v>
       </c>
       <c r="B5" s="25">
         <v>64</v>
@@ -5237,7 +5037,7 @@
     </row>
     <row r="6" spans="1:23">
       <c r="A6" t="s">
-        <v>642</v>
+        <v>629</v>
       </c>
       <c r="B6" s="25">
         <v>61</v>
@@ -5247,14 +5047,14 @@
       <c r="A7" t="s">
         <v>363</v>
       </c>
-      <c r="B7" s="49">
+      <c r="B7" s="48">
         <f>B5+B6</f>
         <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:23">
       <c r="A8" t="s">
-        <v>490</v>
+        <v>477</v>
       </c>
       <c r="B8" s="25">
         <v>200</v>
@@ -5262,7 +5062,7 @@
     </row>
     <row r="9" spans="1:23">
       <c r="A9" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
       <c r="B9" s="25">
         <v>4</v>
@@ -5270,7 +5070,7 @@
     </row>
     <row r="10" spans="1:23">
       <c r="A10" t="s">
-        <v>495</v>
+        <v>482</v>
       </c>
       <c r="B10" s="25">
         <v>12</v>
@@ -5284,27 +5084,27 @@
     </row>
     <row r="11" spans="1:23">
       <c r="A11" t="s">
-        <v>497</v>
-      </c>
-      <c r="B11" s="97">
+        <v>484</v>
+      </c>
+      <c r="B11" s="96">
         <f>B8 / (B9*B10)</f>
         <v>4.166666666666667</v>
       </c>
     </row>
     <row r="12" spans="1:23">
       <c r="A12" t="s">
-        <v>496</v>
-      </c>
-      <c r="B12" s="49">
+        <v>483</v>
+      </c>
+      <c r="B12" s="48">
         <f>B9-B1</f>
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:23">
       <c r="A13" t="s">
-        <v>498</v>
-      </c>
-      <c r="B13" s="49">
+        <v>485</v>
+      </c>
+      <c r="B13" s="48">
         <f>(gsPeriodsLeft*gsMinsPerPeriod)+gsMins+ csSecs/60</f>
         <v>24</v>
       </c>
@@ -5315,62 +5115,62 @@
     </row>
     <row r="14" spans="1:23">
       <c r="A14" t="s">
-        <v>499</v>
-      </c>
-      <c r="B14" s="49">
+        <v>486</v>
+      </c>
+      <c r="B14" s="48">
         <f>B13*B11 + B7</f>
         <v>225</v>
       </c>
       <c r="C14" t="s">
-        <v>618</v>
-      </c>
-      <c r="W14" s="50" t="s">
-        <v>500</v>
+        <v>605</v>
+      </c>
+      <c r="W14" s="49" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="15" spans="1:23">
       <c r="A15" t="s">
-        <v>644</v>
-      </c>
-      <c r="B15" s="49">
+        <v>631</v>
+      </c>
+      <c r="B15" s="48">
         <f>IF(B7&gt;B8,"OVER",B14-B8)</f>
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" t="s">
-        <v>502</v>
+        <v>489</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>501</v>
+        <v>488</v>
       </c>
       <c r="B19" t="s">
-        <v>503</v>
+        <v>490</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>504</v>
+        <v>491</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="B22" t="s">
-        <v>505</v>
+        <v>492</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="B23" t="s">
-        <v>506</v>
+        <v>493</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>507</v>
+        <v>494</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -5380,48 +5180,48 @@
     </row>
     <row r="27" spans="1:5">
       <c r="B27" t="s">
-        <v>508</v>
+        <v>495</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="B30" t="s">
-        <v>510</v>
+        <v>497</v>
       </c>
       <c r="C30" t="s">
         <v>467</v>
       </c>
       <c r="D30" t="s">
-        <v>509</v>
+        <v>496</v>
       </c>
       <c r="E30" t="s">
-        <v>508</v>
+        <v>495</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="B33" t="s">
-        <v>651</v>
+        <v>638</v>
       </c>
       <c r="C33" t="s">
-        <v>652</v>
+        <v>639</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="B34" s="80">
+      <c r="B34" s="79">
         <v>1</v>
       </c>
-      <c r="C34" s="80">
+      <c r="C34" s="79">
         <v>2</v>
       </c>
-      <c r="D34" s="80">
+      <c r="D34" s="79">
         <v>3</v>
       </c>
-      <c r="E34" s="80">
+      <c r="E34" s="79">
         <v>4</v>
       </c>
-      <c r="F34" s="80">
+      <c r="F34" s="79">
         <v>5</v>
       </c>
-      <c r="G34" s="80">
+      <c r="G34" s="79">
         <v>6</v>
       </c>
     </row>
@@ -5442,228 +5242,228 @@
         <v>455</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>625</v>
+        <v>612</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>646</v>
-      </c>
-      <c r="B36" s="81">
+        <v>633</v>
+      </c>
+      <c r="B36" s="80">
         <v>603</v>
       </c>
-      <c r="C36" s="82" t="s">
-        <v>621</v>
-      </c>
-      <c r="D36" s="82" t="s">
+      <c r="C36" s="81" t="s">
+        <v>608</v>
+      </c>
+      <c r="D36" s="81" t="s">
         <v>374</v>
       </c>
-      <c r="E36" s="82">
+      <c r="E36" s="81">
         <v>100</v>
       </c>
-      <c r="F36" s="83" t="s">
-        <v>622</v>
-      </c>
-      <c r="G36" s="84"/>
+      <c r="F36" s="82" t="s">
+        <v>609</v>
+      </c>
+      <c r="G36" s="83"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="B37" s="85" t="s">
-        <v>619</v>
-      </c>
-      <c r="C37" s="86" t="s">
-        <v>620</v>
-      </c>
-      <c r="D37" s="86">
+      <c r="B37" s="84" t="s">
+        <v>606</v>
+      </c>
+      <c r="C37" s="85" t="s">
+        <v>607</v>
+      </c>
+      <c r="D37" s="85">
         <v>220</v>
       </c>
-      <c r="E37" s="86">
+      <c r="E37" s="85">
         <v>105</v>
       </c>
-      <c r="F37" s="87" t="s">
-        <v>623</v>
-      </c>
-      <c r="G37" s="88" t="s">
-        <v>624</v>
+      <c r="F37" s="86" t="s">
+        <v>610</v>
+      </c>
+      <c r="G37" s="87" t="s">
+        <v>611</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>645</v>
-      </c>
-      <c r="B38" s="81">
+        <v>632</v>
+      </c>
+      <c r="B38" s="80">
         <v>603</v>
       </c>
-      <c r="C38" s="82" t="s">
-        <v>621</v>
-      </c>
-      <c r="D38" s="82" t="s">
-        <v>626</v>
-      </c>
-      <c r="E38" s="82"/>
-      <c r="F38" s="83"/>
-      <c r="G38" s="89" t="s">
-        <v>627</v>
+      <c r="C38" s="81" t="s">
+        <v>608</v>
+      </c>
+      <c r="D38" s="81" t="s">
+        <v>613</v>
+      </c>
+      <c r="E38" s="81"/>
+      <c r="F38" s="82"/>
+      <c r="G38" s="88" t="s">
+        <v>614</v>
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="B39" s="85" t="s">
-        <v>627</v>
-      </c>
-      <c r="C39" s="86" t="s">
-        <v>620</v>
-      </c>
-      <c r="D39" s="86">
+      <c r="B39" s="84" t="s">
+        <v>614</v>
+      </c>
+      <c r="C39" s="85" t="s">
+        <v>607</v>
+      </c>
+      <c r="D39" s="85">
         <v>220</v>
       </c>
-      <c r="E39" s="86"/>
-      <c r="F39" s="87"/>
-      <c r="G39" s="88" t="s">
-        <v>628</v>
+      <c r="E39" s="85"/>
+      <c r="F39" s="86"/>
+      <c r="G39" s="87" t="s">
+        <v>615</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>648</v>
-      </c>
-      <c r="B40" s="81">
+        <v>635</v>
+      </c>
+      <c r="B40" s="80">
         <v>603</v>
       </c>
-      <c r="C40" s="82" t="s">
-        <v>621</v>
-      </c>
-      <c r="D40" s="82" t="s">
-        <v>626</v>
-      </c>
-      <c r="E40" s="82"/>
-      <c r="F40" s="83"/>
-      <c r="G40" s="89" t="s">
-        <v>648</v>
+      <c r="C40" s="81" t="s">
+        <v>608</v>
+      </c>
+      <c r="D40" s="81" t="s">
+        <v>613</v>
+      </c>
+      <c r="E40" s="81"/>
+      <c r="F40" s="82"/>
+      <c r="G40" s="88" t="s">
+        <v>635</v>
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="B41" s="85" t="s">
-        <v>627</v>
-      </c>
-      <c r="C41" s="86" t="s">
-        <v>620</v>
-      </c>
-      <c r="D41" s="86">
+      <c r="B41" s="84" t="s">
+        <v>614</v>
+      </c>
+      <c r="C41" s="85" t="s">
+        <v>607</v>
+      </c>
+      <c r="D41" s="85">
         <v>220</v>
       </c>
-      <c r="E41" s="86"/>
-      <c r="F41" s="87"/>
-      <c r="G41" s="88"/>
+      <c r="E41" s="85"/>
+      <c r="F41" s="86"/>
+      <c r="G41" s="87"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>578</v>
-      </c>
-      <c r="B42" s="81">
+        <v>565</v>
+      </c>
+      <c r="B42" s="80">
         <v>603</v>
       </c>
-      <c r="C42" s="82" t="s">
-        <v>621</v>
-      </c>
-      <c r="D42" s="82" t="s">
+      <c r="C42" s="81" t="s">
+        <v>608</v>
+      </c>
+      <c r="D42" s="81" t="s">
         <v>374</v>
       </c>
-      <c r="E42" s="82">
+      <c r="E42" s="81">
         <v>100</v>
       </c>
-      <c r="F42" s="83" t="s">
-        <v>578</v>
-      </c>
-      <c r="G42" s="84"/>
-      <c r="H42" s="98" t="s">
-        <v>647</v>
+      <c r="F42" s="82" t="s">
+        <v>565</v>
+      </c>
+      <c r="G42" s="83"/>
+      <c r="H42" s="97" t="s">
+        <v>634</v>
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="B43" s="85" t="s">
-        <v>619</v>
-      </c>
-      <c r="C43" s="86" t="s">
-        <v>620</v>
-      </c>
-      <c r="D43" s="86">
+      <c r="B43" s="84" t="s">
+        <v>606</v>
+      </c>
+      <c r="C43" s="85" t="s">
+        <v>607</v>
+      </c>
+      <c r="D43" s="85">
         <v>220</v>
       </c>
-      <c r="E43" s="86">
+      <c r="E43" s="85">
         <v>105</v>
       </c>
-      <c r="F43" s="87" t="s">
-        <v>626</v>
-      </c>
-      <c r="G43" s="88" t="s">
-        <v>629</v>
+      <c r="F43" s="86" t="s">
+        <v>613</v>
+      </c>
+      <c r="G43" s="87" t="s">
+        <v>616</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="30">
       <c r="A44" t="s">
-        <v>649</v>
-      </c>
-      <c r="B44" s="90" t="s">
+        <v>636</v>
+      </c>
+      <c r="B44" s="89" t="s">
         <v>378</v>
       </c>
-      <c r="C44" s="91" t="s">
-        <v>636</v>
-      </c>
-      <c r="D44" s="91" t="s">
-        <v>630</v>
-      </c>
-      <c r="E44" s="91" t="s">
-        <v>631</v>
-      </c>
-      <c r="F44" s="92" t="s">
-        <v>633</v>
-      </c>
-      <c r="G44" s="90" t="s">
+      <c r="C44" s="90" t="s">
+        <v>623</v>
+      </c>
+      <c r="D44" s="90" t="s">
+        <v>617</v>
+      </c>
+      <c r="E44" s="90" t="s">
+        <v>618</v>
+      </c>
+      <c r="F44" s="91" t="s">
+        <v>620</v>
+      </c>
+      <c r="G44" s="89" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="30">
+      <c r="B45" s="91" t="s">
+        <v>622</v>
+      </c>
+      <c r="C45" s="90" t="s">
+        <v>624</v>
+      </c>
+      <c r="D45" s="89" t="s">
+        <v>72</v>
+      </c>
+      <c r="E45" s="90" t="s">
+        <v>619</v>
+      </c>
+      <c r="F45" s="91" t="s">
+        <v>621</v>
+      </c>
+      <c r="G45" s="90" t="s">
         <v>625</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="30">
-      <c r="B45" s="92" t="s">
-        <v>635</v>
-      </c>
-      <c r="C45" s="91" t="s">
-        <v>637</v>
-      </c>
-      <c r="D45" s="90" t="s">
-        <v>72</v>
-      </c>
-      <c r="E45" s="91" t="s">
-        <v>632</v>
-      </c>
-      <c r="F45" s="92" t="s">
-        <v>634</v>
-      </c>
-      <c r="G45" s="91" t="s">
-        <v>638</v>
-      </c>
-    </row>
     <row r="48" spans="1:8">
-      <c r="B48" s="80">
+      <c r="B48" s="79">
         <v>1</v>
       </c>
-      <c r="C48" s="80">
+      <c r="C48" s="79">
         <v>2</v>
       </c>
-      <c r="D48" s="80">
+      <c r="D48" s="79">
         <v>3</v>
       </c>
-      <c r="E48" s="80">
+      <c r="E48" s="79">
         <v>4</v>
       </c>
-      <c r="F48" s="80">
+      <c r="F48" s="79">
         <v>5</v>
       </c>
-      <c r="G48" s="80">
+      <c r="G48" s="79">
         <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>650</v>
+        <v>637</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>372</v>
@@ -5681,94 +5481,94 @@
         <v>455</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>625</v>
+        <v>612</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>646</v>
-      </c>
-      <c r="B50" s="93">
+        <v>633</v>
+      </c>
+      <c r="B50" s="92">
         <v>603</v>
       </c>
-      <c r="C50" s="94" t="s">
-        <v>621</v>
-      </c>
-      <c r="D50" s="94" t="s">
-        <v>639</v>
-      </c>
-      <c r="E50" s="94">
+      <c r="C50" s="93" t="s">
+        <v>608</v>
+      </c>
+      <c r="D50" s="93" t="s">
+        <v>626</v>
+      </c>
+      <c r="E50" s="93">
         <v>115</v>
       </c>
-      <c r="F50" s="95" t="s">
-        <v>622</v>
-      </c>
-      <c r="G50" s="96" t="s">
-        <v>624</v>
+      <c r="F50" s="94" t="s">
+        <v>609</v>
+      </c>
+      <c r="G50" s="95" t="s">
+        <v>611</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>645</v>
-      </c>
-      <c r="B51" s="93">
+        <v>632</v>
+      </c>
+      <c r="B51" s="92">
         <v>603</v>
       </c>
-      <c r="C51" s="94" t="s">
-        <v>621</v>
-      </c>
-      <c r="D51" s="94" t="s">
-        <v>639</v>
-      </c>
-      <c r="E51" s="94" t="s">
-        <v>640</v>
-      </c>
-      <c r="F51" s="85" t="s">
+      <c r="C51" s="93" t="s">
+        <v>608</v>
+      </c>
+      <c r="D51" s="93" t="s">
+        <v>626</v>
+      </c>
+      <c r="E51" s="93" t="s">
         <v>627</v>
       </c>
-      <c r="G51" s="96" t="s">
-        <v>628</v>
+      <c r="F51" s="84" t="s">
+        <v>614</v>
+      </c>
+      <c r="G51" s="95" t="s">
+        <v>615</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>648</v>
-      </c>
-      <c r="B52" s="93">
+        <v>635</v>
+      </c>
+      <c r="B52" s="92">
         <v>603</v>
       </c>
-      <c r="C52" s="94" t="s">
-        <v>621</v>
-      </c>
-      <c r="D52" s="94" t="s">
-        <v>639</v>
-      </c>
-      <c r="E52" s="94"/>
-      <c r="F52" s="85"/>
-      <c r="G52" s="89" t="s">
-        <v>648</v>
+      <c r="C52" s="93" t="s">
+        <v>608</v>
+      </c>
+      <c r="D52" s="93" t="s">
+        <v>626</v>
+      </c>
+      <c r="E52" s="93"/>
+      <c r="F52" s="84"/>
+      <c r="G52" s="88" t="s">
+        <v>635</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>578</v>
-      </c>
-      <c r="B53" s="93">
+        <v>565</v>
+      </c>
+      <c r="B53" s="92">
         <v>603</v>
       </c>
-      <c r="C53" s="94" t="s">
-        <v>621</v>
-      </c>
-      <c r="D53" s="94" t="s">
-        <v>639</v>
-      </c>
-      <c r="E53" s="94">
+      <c r="C53" s="93" t="s">
+        <v>608</v>
+      </c>
+      <c r="D53" s="93" t="s">
+        <v>626</v>
+      </c>
+      <c r="E53" s="93">
         <v>222</v>
       </c>
-      <c r="F53" s="85" t="s">
-        <v>578</v>
-      </c>
-      <c r="G53" s="96" t="s">
+      <c r="F53" s="84" t="s">
+        <v>565</v>
+      </c>
+      <c r="G53" s="95" t="s">
         <v>375</v>
       </c>
     </row>
@@ -5779,7 +5579,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA054234-7E0D-4664-8686-43EE406DF08B}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:E5"/>
@@ -5877,7 +5677,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56197CAD-6F82-4F44-8E32-9D17A9159C60}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:O5"/>
@@ -5893,11 +5693,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="J1" s="99" t="s">
+      <c r="J1" s="98" t="s">
         <v>368</v>
       </c>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
@@ -5947,7 +5747,7 @@
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -5958,7 +5758,7 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="B4" s="99"/>
+      <c r="B4" s="98"/>
       <c r="C4" s="10" t="s">
         <v>374</v>
       </c>
@@ -5967,7 +5767,7 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="B5" s="99"/>
+      <c r="B5" s="98"/>
       <c r="C5" s="10" t="s">
         <v>375</v>
       </c>
@@ -5984,7 +5784,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715451AB-D7A2-4155-AA80-E7E1839EA9EB}">
   <sheetPr codeName="Sheet17" filterMode="1"/>
   <dimension ref="A1:E95"/>
@@ -6001,20 +5801,20 @@
     <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="56" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:5" s="55" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A1" s="56" t="s">
         <v>247</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="56" t="s">
         <v>248</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="56" t="s">
         <v>249</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="56" t="s">
         <v>250</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="57" t="s">
         <v>330</v>
       </c>
     </row>
@@ -7467,7 +7267,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A5C7EC-EF5B-47DA-AE1B-CF3EEA06F69E}">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -7482,7 +7282,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>614</v>
+        <v>601</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -7492,7 +7292,7 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>615</v>
+        <v>602</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -7510,7 +7310,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB6D801-3E13-4E99-8E4E-00DE466D45BE}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A2:C5"/>
@@ -7564,6 +7364,175 @@
       </c>
       <c r="C5" t="s">
         <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F968386-0DC8-4BEE-BB1E-0C17B7C52875}">
+  <sheetPr codeName="Sheet18"/>
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>446</v>
+      </c>
+      <c r="B2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C2" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <f>A3*B3</f>
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>13.74</v>
+      </c>
+      <c r="E3">
+        <v>16.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <f>A4*B4</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <f>A5*B5</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>447</v>
+      </c>
+      <c r="B6" t="s">
+        <v>451</v>
+      </c>
+      <c r="C6">
+        <f>SUM(C3:C5)</f>
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>73.3</v>
+      </c>
+      <c r="E6">
+        <v>82.584999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>450</v>
+      </c>
+      <c r="C7">
+        <v>-0.5</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>453</v>
+      </c>
+      <c r="C8">
+        <f>(C6+C7) / C6</f>
+        <v>0.995</v>
+      </c>
+      <c r="D8">
+        <f>(D6+D7) / D6</f>
+        <v>1.0272851296043657</v>
+      </c>
+      <c r="E8">
+        <f>(E6+E7) / E6</f>
+        <v>1.0242174729067022</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <f>C3*C$8</f>
+        <v>19.899999999999999</v>
+      </c>
+      <c r="D10">
+        <f>D3*D$8</f>
+        <v>14.114897680763985</v>
+      </c>
+      <c r="E10">
+        <f>E3*E$8</f>
+        <v>17.155642671187262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <f>C4*C$8</f>
+        <v>49.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <f>C5*C$8</f>
+        <v>29.85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="C13">
+        <f>SUM(C10:C12)</f>
+        <v>99.5</v>
       </c>
     </row>
   </sheetData>
@@ -7617,175 +7586,6 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F968386-0DC8-4BEE-BB1E-0C17B7C52875}">
-  <sheetPr codeName="Sheet18"/>
-  <dimension ref="A1:E13"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="B1" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>446</v>
-      </c>
-      <c r="B2" t="s">
-        <v>351</v>
-      </c>
-      <c r="C2" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>20</v>
-      </c>
-      <c r="C3">
-        <f>A3*B3</f>
-        <v>20</v>
-      </c>
-      <c r="D3">
-        <v>13.74</v>
-      </c>
-      <c r="E3">
-        <v>16.75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>25</v>
-      </c>
-      <c r="C4">
-        <f>A4*B4</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <f>A5*B5</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>447</v>
-      </c>
-      <c r="B6" t="s">
-        <v>451</v>
-      </c>
-      <c r="C6">
-        <f>SUM(C3:C5)</f>
-        <v>100</v>
-      </c>
-      <c r="D6">
-        <v>73.3</v>
-      </c>
-      <c r="E6">
-        <v>82.584999999999994</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>450</v>
-      </c>
-      <c r="C7">
-        <v>-0.5</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>453</v>
-      </c>
-      <c r="C8">
-        <f>(C6+C7) / C6</f>
-        <v>0.995</v>
-      </c>
-      <c r="D8">
-        <f>(D6+D7) / D6</f>
-        <v>1.0272851296043657</v>
-      </c>
-      <c r="E8">
-        <f>(E6+E7) / E6</f>
-        <v>1.0242174729067022</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <f>C3*C$8</f>
-        <v>19.899999999999999</v>
-      </c>
-      <c r="D10">
-        <f>D3*D$8</f>
-        <v>14.114897680763985</v>
-      </c>
-      <c r="E10">
-        <f>E3*E$8</f>
-        <v>17.155642671187262</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <f>C4*C$8</f>
-        <v>49.75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <f>C5*C$8</f>
-        <v>29.85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="C13">
-        <f>SUM(C10:C12)</f>
-        <v>99.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{171E99EC-4E48-4A0D-9949-97CC135E53EA}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1"/>
@@ -7801,7 +7601,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F22086FA-BC76-4860-9395-82D35EE90630}">
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A2:B62"/>
@@ -8166,12 +7966,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A09DBAA-B5E4-4F0C-9A47-53EEACDA4F1F}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A3:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
@@ -8266,7 +8066,7 @@
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="28" spans="1:3" ht="11.25" customHeight="1">
-      <c r="A28" s="100" t="s">
+      <c r="A28" s="99" t="s">
         <v>69</v>
       </c>
       <c r="B28" s="19" t="s">
@@ -8277,7 +8077,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="12" customHeight="1">
-      <c r="A29" s="101"/>
+      <c r="A29" s="100"/>
       <c r="B29" s="20" t="s">
         <v>72</v>
       </c>
@@ -8286,14 +8086,14 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A30" s="101"/>
+      <c r="A30" s="100"/>
       <c r="B30" s="21"/>
       <c r="C30" s="24" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A31" s="102"/>
+      <c r="A31" s="101"/>
       <c r="B31" s="18"/>
       <c r="C31" s="17" t="s">
         <v>70</v>
@@ -9031,41 +8831,41 @@
     <col min="22" max="22" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="56" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A1" s="54" t="s">
-        <v>511</v>
-      </c>
-      <c r="B1" s="54" t="s">
+    <row r="1" spans="1:22" s="55" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A1" s="53" t="s">
+        <v>498</v>
+      </c>
+      <c r="B1" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="53" t="s">
         <v>227</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="53" t="s">
         <v>444</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="53" t="s">
         <v>450</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="53" t="s">
         <v>343</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="54" t="s">
         <v>344</v>
       </c>
-      <c r="I1" s="56" t="str">
+      <c r="I1" s="55" t="str">
         <f>"SELECT  max(GameDate) as " &amp; D1 &amp; "MaxDate FROM " &amp; D1</f>
         <v>SELECT  max(GameDate) as Table OutMaxDate FROM Table Out</v>
       </c>
     </row>
     <row r="2" spans="1:22">
-      <c r="A2" s="51">
+      <c r="A2" s="50">
         <v>1</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="50" t="s">
         <v>205</v>
       </c>
     </row>
@@ -9085,7 +8885,7 @@
     </row>
     <row r="4" spans="1:22">
       <c r="B4" s="32" t="s">
-        <v>616</v>
+        <v>603</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s">
@@ -9097,7 +8897,7 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="B5" t="s">
-        <v>481</v>
+        <v>468</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -9164,8 +8964,8 @@
       </c>
     </row>
     <row r="12" spans="1:22">
-      <c r="B12" s="77" t="s">
-        <v>594</v>
+      <c r="B12" s="76" t="s">
+        <v>581</v>
       </c>
       <c r="E12">
         <v>0.2</v>
@@ -9175,16 +8975,16 @@
       </c>
     </row>
     <row r="13" spans="1:22">
-      <c r="B13" s="77" t="s">
-        <v>595</v>
+      <c r="B13" s="76" t="s">
+        <v>582</v>
       </c>
       <c r="E13">
         <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:22">
-      <c r="B14" s="77" t="s">
-        <v>596</v>
+      <c r="B14" s="76" t="s">
+        <v>583</v>
       </c>
       <c r="E14">
         <v>0.67</v>
@@ -9197,7 +8997,7 @@
     </row>
     <row r="16" spans="1:22">
       <c r="B16" s="13" t="s">
-        <v>539</v>
+        <v>526</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30">
@@ -9214,7 +9014,7 @@
     </row>
     <row r="19" spans="1:11">
       <c r="B19" s="3" t="s">
-        <v>487</v>
+        <v>474</v>
       </c>
       <c r="C19" s="3"/>
     </row>
@@ -9223,14 +9023,14 @@
         <v>1.41</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>488</v>
+        <v>475</v>
       </c>
       <c r="C20" s="3"/>
       <c r="E20" t="s">
         <v>450</v>
       </c>
       <c r="F20" t="s">
-        <v>487</v>
+        <v>474</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -9298,7 +9098,7 @@
         <v>361</v>
       </c>
       <c r="H27" s="43" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -9334,7 +9134,7 @@
         <v>198</v>
       </c>
       <c r="G29" s="13"/>
-      <c r="H29" s="48"/>
+      <c r="H29" s="47"/>
     </row>
     <row r="30" spans="1:11">
       <c r="B30" s="2" t="s">
@@ -9345,7 +9145,7 @@
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
-      <c r="H30" s="48"/>
+      <c r="H30" s="47"/>
       <c r="K30" t="s">
         <v>246</v>
       </c>
@@ -9371,7 +9171,7 @@
         <v>450</v>
       </c>
       <c r="F32" t="s">
-        <v>485</v>
+        <v>472</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -9383,7 +9183,7 @@
       </c>
       <c r="C33" s="30"/>
       <c r="H33" s="43" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -9408,10 +9208,10 @@
         <v>450</v>
       </c>
       <c r="F36" t="s">
-        <v>486</v>
+        <v>473</v>
       </c>
       <c r="H36" s="43" t="s">
-        <v>484</v>
+        <v>471</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -9426,7 +9226,7 @@
         <v>45</v>
       </c>
       <c r="E37" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
@@ -9434,7 +9234,7 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="33" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>354</v>
@@ -9444,12 +9244,12 @@
         <v>186</v>
       </c>
       <c r="E38" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="33" t="s">
-        <v>607</v>
+        <v>594</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>197</v>
@@ -9458,28 +9258,28 @@
         <v>186</v>
       </c>
       <c r="E39" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="33" t="s">
-        <v>612</v>
+        <v>599</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>613</v>
+        <v>600</v>
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="51">
+      <c r="A41" s="50">
         <v>2</v>
       </c>
-      <c r="B41" s="52"/>
+      <c r="B41" s="51"/>
       <c r="C41" s="2"/>
       <c r="E41" t="s">
         <v>355</v>
       </c>
       <c r="F41" t="s">
-        <v>489</v>
+        <v>476</v>
       </c>
       <c r="G41" s="13" t="s">
         <v>340</v>
@@ -9533,7 +9333,7 @@
         <v>46</v>
       </c>
       <c r="E46" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -9542,7 +9342,7 @@
       </c>
       <c r="C47" s="5"/>
       <c r="E47" t="s">
-        <v>525</v>
+        <v>512</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -9552,10 +9352,10 @@
       <c r="C48" s="5"/>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="51">
+      <c r="A49" s="50">
         <v>3</v>
       </c>
-      <c r="B49" s="53" t="s">
+      <c r="B49" s="52" t="s">
         <v>211</v>
       </c>
       <c r="C49" s="32"/>
@@ -9655,10 +9455,10 @@
       <c r="C60" s="35"/>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61" s="51">
+      <c r="A61" s="50">
         <v>4</v>
       </c>
-      <c r="B61" s="53" t="s">
+      <c r="B61" s="52" t="s">
         <v>232</v>
       </c>
     </row>
@@ -9771,7 +9571,7 @@
         <v>4.3499999999999996</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>574</v>
+        <v>561</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="14"/>
@@ -9781,8 +9581,8 @@
       <c r="H73" s="14"/>
     </row>
     <row r="74" spans="1:11">
-      <c r="B74" s="61" t="s">
-        <v>575</v>
+      <c r="B74" s="60" t="s">
+        <v>562</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="14"/>
@@ -9792,8 +9592,8 @@
       <c r="H74" s="14"/>
     </row>
     <row r="75" spans="1:11">
-      <c r="B75" s="61" t="s">
-        <v>576</v>
+      <c r="B75" s="60" t="s">
+        <v>563</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="14"/>
@@ -9803,8 +9603,8 @@
       <c r="H75" s="14"/>
     </row>
     <row r="76" spans="1:11">
-      <c r="B76" s="61" t="s">
-        <v>577</v>
+      <c r="B76" s="60" t="s">
+        <v>564</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="14"/>
@@ -9818,7 +9618,7 @@
         <v>4.3499999999999996</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>555</v>
+        <v>542</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="14"/>
@@ -9828,8 +9628,8 @@
       <c r="H77" s="14"/>
     </row>
     <row r="78" spans="1:11">
-      <c r="B78" s="65" t="s">
-        <v>556</v>
+      <c r="B78" s="64" t="s">
+        <v>543</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="14"/>
@@ -9839,8 +9639,8 @@
       <c r="H78" s="14"/>
     </row>
     <row r="79" spans="1:11">
-      <c r="B79" s="65" t="s">
-        <v>557</v>
+      <c r="B79" s="64" t="s">
+        <v>544</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="14"/>
@@ -9850,8 +9650,8 @@
       <c r="H79" s="14"/>
     </row>
     <row r="80" spans="1:11">
-      <c r="B80" s="65" t="s">
-        <v>558</v>
+      <c r="B80" s="64" t="s">
+        <v>545</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="14"/>
@@ -9861,8 +9661,8 @@
       <c r="H80" s="14"/>
     </row>
     <row r="81" spans="2:8">
-      <c r="B81" s="65" t="s">
-        <v>559</v>
+      <c r="B81" s="64" t="s">
+        <v>546</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="14"/>
@@ -9872,8 +9672,8 @@
       <c r="H81" s="14"/>
     </row>
     <row r="82" spans="2:8">
-      <c r="B82" s="65" t="s">
-        <v>560</v>
+      <c r="B82" s="64" t="s">
+        <v>547</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="14"/>
@@ -9883,8 +9683,8 @@
       <c r="H82" s="14"/>
     </row>
     <row r="83" spans="2:8">
-      <c r="B83" s="65" t="s">
-        <v>561</v>
+      <c r="B83" s="64" t="s">
+        <v>548</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="14"/>
@@ -9894,8 +9694,8 @@
       <c r="H83" s="14"/>
     </row>
     <row r="84" spans="2:8">
-      <c r="B84" s="66" t="s">
-        <v>562</v>
+      <c r="B84" s="65" t="s">
+        <v>549</v>
       </c>
       <c r="C84" s="14"/>
       <c r="D84" s="14"/>
@@ -9904,11 +9704,11 @@
       <c r="H84"/>
     </row>
     <row r="85" spans="2:8">
-      <c r="B85" s="66" t="s">
-        <v>563</v>
+      <c r="B85" s="65" t="s">
+        <v>550</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>564</v>
+        <v>551</v>
       </c>
       <c r="D85" s="14"/>
       <c r="E85" s="14"/>
@@ -9916,8 +9716,8 @@
       <c r="H85"/>
     </row>
     <row r="86" spans="2:8">
-      <c r="B86" s="66" t="s">
-        <v>565</v>
+      <c r="B86" s="65" t="s">
+        <v>552</v>
       </c>
       <c r="C86" s="14"/>
       <c r="D86" s="14"/>
@@ -9926,8 +9726,8 @@
       <c r="H86"/>
     </row>
     <row r="87" spans="2:8">
-      <c r="B87" s="65" t="s">
-        <v>566</v>
+      <c r="B87" s="64" t="s">
+        <v>553</v>
       </c>
       <c r="C87" s="14"/>
       <c r="D87" s="14"/>
@@ -9937,8 +9737,8 @@
       <c r="H87"/>
     </row>
     <row r="88" spans="2:8">
-      <c r="B88" s="65" t="s">
-        <v>567</v>
+      <c r="B88" s="64" t="s">
+        <v>554</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="14"/>
@@ -9948,8 +9748,8 @@
       <c r="H88" s="14"/>
     </row>
     <row r="89" spans="2:8">
-      <c r="B89" s="66" t="s">
-        <v>562</v>
+      <c r="B89" s="65" t="s">
+        <v>549</v>
       </c>
       <c r="C89" s="14"/>
       <c r="D89" s="14"/>
@@ -9958,11 +9758,11 @@
       <c r="H89"/>
     </row>
     <row r="90" spans="2:8">
-      <c r="B90" s="66" t="s">
-        <v>568</v>
+      <c r="B90" s="65" t="s">
+        <v>555</v>
       </c>
       <c r="C90" s="14" t="s">
-        <v>564</v>
+        <v>551</v>
       </c>
       <c r="D90" s="14"/>
       <c r="E90" s="14"/>
@@ -9970,8 +9770,8 @@
       <c r="H90"/>
     </row>
     <row r="91" spans="2:8">
-      <c r="B91" s="66" t="s">
-        <v>569</v>
+      <c r="B91" s="65" t="s">
+        <v>556</v>
       </c>
       <c r="C91" s="14"/>
       <c r="D91" s="14"/>
@@ -9980,8 +9780,8 @@
       <c r="H91"/>
     </row>
     <row r="92" spans="2:8">
-      <c r="B92" s="66" t="s">
-        <v>570</v>
+      <c r="B92" s="65" t="s">
+        <v>557</v>
       </c>
       <c r="C92" s="14"/>
       <c r="D92" s="14"/>
@@ -9990,8 +9790,8 @@
       <c r="H92"/>
     </row>
     <row r="93" spans="2:8">
-      <c r="B93" s="66" t="s">
-        <v>571</v>
+      <c r="B93" s="65" t="s">
+        <v>558</v>
       </c>
       <c r="C93" s="14"/>
       <c r="D93" s="14"/>
@@ -10000,8 +9800,8 @@
       <c r="H93"/>
     </row>
     <row r="94" spans="2:8">
-      <c r="B94" s="65" t="s">
-        <v>572</v>
+      <c r="B94" s="64" t="s">
+        <v>559</v>
       </c>
       <c r="D94" s="14"/>
       <c r="E94" s="14"/>
@@ -10010,8 +9810,8 @@
       <c r="H94" s="14"/>
     </row>
     <row r="95" spans="2:8">
-      <c r="B95" s="65" t="s">
-        <v>573</v>
+      <c r="B95" s="64" t="s">
+        <v>560</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="14"/>
@@ -10043,7 +9843,7 @@
         <v>4.3499999999999996</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>544</v>
+        <v>531</v>
       </c>
       <c r="C98" s="1"/>
       <c r="D98" s="14"/>
@@ -10053,109 +9853,109 @@
       <c r="H98" s="14"/>
     </row>
     <row r="99" spans="1:9">
-      <c r="B99" s="61" t="s">
-        <v>545</v>
-      </c>
-      <c r="C99" s="61"/>
-      <c r="D99" s="62"/>
-      <c r="E99" s="62"/>
-      <c r="F99" s="62"/>
-      <c r="G99" s="62"/>
-      <c r="H99" s="62"/>
-      <c r="I99" s="63"/>
+      <c r="B99" s="60" t="s">
+        <v>532</v>
+      </c>
+      <c r="C99" s="60"/>
+      <c r="D99" s="61"/>
+      <c r="E99" s="61"/>
+      <c r="F99" s="61"/>
+      <c r="G99" s="61"/>
+      <c r="H99" s="61"/>
+      <c r="I99" s="62"/>
     </row>
     <row r="100" spans="1:9">
-      <c r="B100" s="61" t="s">
-        <v>553</v>
-      </c>
-      <c r="D100" s="62"/>
-      <c r="E100" s="62"/>
-      <c r="F100" s="62"/>
-      <c r="G100" s="62"/>
-      <c r="H100" s="62"/>
-      <c r="I100" s="63"/>
+      <c r="B100" s="60" t="s">
+        <v>540</v>
+      </c>
+      <c r="D100" s="61"/>
+      <c r="E100" s="61"/>
+      <c r="F100" s="61"/>
+      <c r="G100" s="61"/>
+      <c r="H100" s="61"/>
+      <c r="I100" s="62"/>
     </row>
     <row r="101" spans="1:9">
-      <c r="B101" s="61" t="s">
-        <v>546</v>
-      </c>
-      <c r="C101" s="61"/>
-      <c r="D101" s="62"/>
-      <c r="E101" s="62"/>
-      <c r="F101" s="62"/>
-      <c r="G101" s="62"/>
-      <c r="H101" s="62"/>
-      <c r="I101" s="63"/>
+      <c r="B101" s="60" t="s">
+        <v>533</v>
+      </c>
+      <c r="C101" s="60"/>
+      <c r="D101" s="61"/>
+      <c r="E101" s="61"/>
+      <c r="F101" s="61"/>
+      <c r="G101" s="61"/>
+      <c r="H101" s="61"/>
+      <c r="I101" s="62"/>
     </row>
     <row r="102" spans="1:9">
-      <c r="B102" s="61" t="s">
-        <v>547</v>
-      </c>
-      <c r="C102" s="61"/>
-      <c r="D102" s="62"/>
-      <c r="E102" s="62"/>
-      <c r="F102" s="62"/>
-      <c r="G102" s="62"/>
-      <c r="H102" s="62"/>
-      <c r="I102" s="63"/>
+      <c r="B102" s="60" t="s">
+        <v>534</v>
+      </c>
+      <c r="C102" s="60"/>
+      <c r="D102" s="61"/>
+      <c r="E102" s="61"/>
+      <c r="F102" s="61"/>
+      <c r="G102" s="61"/>
+      <c r="H102" s="61"/>
+      <c r="I102" s="62"/>
     </row>
     <row r="103" spans="1:9">
-      <c r="B103" s="62" t="s">
-        <v>548</v>
-      </c>
-      <c r="C103" s="61"/>
-      <c r="E103" s="62"/>
-      <c r="F103" s="62"/>
-      <c r="G103" s="62"/>
-      <c r="H103" s="62"/>
-      <c r="I103" s="63" t="s">
-        <v>549</v>
+      <c r="B103" s="61" t="s">
+        <v>535</v>
+      </c>
+      <c r="C103" s="60"/>
+      <c r="E103" s="61"/>
+      <c r="F103" s="61"/>
+      <c r="G103" s="61"/>
+      <c r="H103" s="61"/>
+      <c r="I103" s="62" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="104" spans="1:9">
-      <c r="B104" s="61" t="s">
-        <v>550</v>
-      </c>
-      <c r="C104" s="61"/>
-      <c r="D104" s="62"/>
-      <c r="E104" s="62"/>
-      <c r="F104" s="62"/>
-      <c r="G104" s="62"/>
-      <c r="H104" s="62"/>
-      <c r="I104" s="63"/>
+      <c r="B104" s="60" t="s">
+        <v>537</v>
+      </c>
+      <c r="C104" s="60"/>
+      <c r="D104" s="61"/>
+      <c r="E104" s="61"/>
+      <c r="F104" s="61"/>
+      <c r="G104" s="61"/>
+      <c r="H104" s="61"/>
+      <c r="I104" s="62"/>
     </row>
     <row r="105" spans="1:9">
-      <c r="B105" s="61" t="s">
-        <v>551</v>
-      </c>
-      <c r="C105" s="61"/>
-      <c r="D105" s="62"/>
-      <c r="E105" s="62"/>
-      <c r="F105" s="62"/>
-      <c r="G105" s="62"/>
-      <c r="H105" s="62"/>
-      <c r="I105" s="63"/>
+      <c r="B105" s="60" t="s">
+        <v>538</v>
+      </c>
+      <c r="C105" s="60"/>
+      <c r="D105" s="61"/>
+      <c r="E105" s="61"/>
+      <c r="F105" s="61"/>
+      <c r="G105" s="61"/>
+      <c r="H105" s="61"/>
+      <c r="I105" s="62"/>
     </row>
     <row r="106" spans="1:9">
-      <c r="B106" s="61" t="s">
-        <v>552</v>
-      </c>
-      <c r="C106" s="61"/>
-      <c r="D106" s="62"/>
-      <c r="E106" s="62"/>
-      <c r="F106" s="64" t="s">
-        <v>554</v>
-      </c>
-      <c r="G106" s="62"/>
-      <c r="H106" s="62"/>
-      <c r="I106" s="63"/>
+      <c r="B106" s="60" t="s">
+        <v>539</v>
+      </c>
+      <c r="C106" s="60"/>
+      <c r="D106" s="61"/>
+      <c r="E106" s="61"/>
+      <c r="F106" s="63" t="s">
+        <v>541</v>
+      </c>
+      <c r="G106" s="61"/>
+      <c r="H106" s="61"/>
+      <c r="I106" s="62"/>
     </row>
     <row r="107" spans="1:9">
       <c r="A107">
         <v>4.3499999999999996</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>540</v>
+        <v>527</v>
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="14"/>
@@ -10165,8 +9965,8 @@
       <c r="H107" s="14"/>
     </row>
     <row r="108" spans="1:9">
-      <c r="B108" s="60" t="s">
-        <v>541</v>
+      <c r="B108" s="59" t="s">
+        <v>528</v>
       </c>
       <c r="C108" s="1"/>
       <c r="D108" s="14"/>
@@ -10176,8 +9976,8 @@
       <c r="H108" s="14"/>
     </row>
     <row r="109" spans="1:9">
-      <c r="B109" s="67" t="s">
-        <v>542</v>
+      <c r="B109" s="66" t="s">
+        <v>529</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="14"/>
@@ -10187,8 +9987,8 @@
       <c r="H109" s="14"/>
     </row>
     <row r="110" spans="1:9">
-      <c r="B110" s="60" t="s">
-        <v>543</v>
+      <c r="B110" s="59" t="s">
+        <v>530</v>
       </c>
       <c r="C110" s="1"/>
       <c r="D110" s="14"/>
@@ -10269,27 +10069,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="C1" s="76" t="s">
-        <v>585</v>
-      </c>
-      <c r="D1" s="76" t="s">
-        <v>586</v>
-      </c>
-      <c r="E1" s="76" t="s">
-        <v>587</v>
+      <c r="C1" s="75" t="s">
+        <v>572</v>
+      </c>
+      <c r="D1" s="75" t="s">
+        <v>573</v>
+      </c>
+      <c r="E1" s="75" t="s">
+        <v>574</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="B2" t="s">
-        <v>597</v>
-      </c>
-      <c r="C2" s="73">
+        <v>584</v>
+      </c>
+      <c r="C2" s="72">
         <v>0.75</v>
       </c>
-      <c r="D2" s="73">
+      <c r="D2" s="72">
         <v>0.2</v>
       </c>
-      <c r="E2" s="73">
+      <c r="E2" s="72">
         <v>0.2</v>
       </c>
     </row>
@@ -10297,68 +10097,68 @@
       <c r="B3" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="73">
+      <c r="C3" s="72">
         <v>0.2</v>
       </c>
-      <c r="D3" s="73">
+      <c r="D3" s="72">
         <v>0.5</v>
       </c>
-      <c r="E3" s="73">
+      <c r="E3" s="72">
         <v>0.67</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="B4" t="s">
-        <v>598</v>
-      </c>
-      <c r="C4" s="73">
+        <v>585</v>
+      </c>
+      <c r="C4" s="72">
         <v>0.75</v>
       </c>
-      <c r="D4" s="73">
+      <c r="D4" s="72">
         <v>0.1</v>
       </c>
-      <c r="E4" s="73">
+      <c r="E4" s="72">
         <v>0.2</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30">
       <c r="B5" s="3" t="s">
-        <v>590</v>
-      </c>
-      <c r="C5" s="74" t="s">
-        <v>599</v>
-      </c>
-      <c r="D5" s="59" t="s">
-        <v>589</v>
+        <v>577</v>
+      </c>
+      <c r="C5" s="73" t="s">
+        <v>586</v>
+      </c>
+      <c r="D5" s="58" t="s">
+        <v>576</v>
       </c>
       <c r="E5" t="s">
-        <v>600</v>
+        <v>587</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="36.75">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="69" t="s">
+        <v>565</v>
+      </c>
+      <c r="B7" s="69" t="s">
+        <v>566</v>
+      </c>
+      <c r="C7" s="70" t="s">
+        <v>567</v>
+      </c>
+      <c r="D7" s="70" t="s">
         <v>578</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="E7" s="69" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="69" t="s">
+        <v>363</v>
+      </c>
+      <c r="G7" s="70" t="s">
         <v>579</v>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="H7" s="74" t="s">
         <v>580</v>
-      </c>
-      <c r="D7" s="71" t="s">
-        <v>591</v>
-      </c>
-      <c r="E7" s="70" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="70" t="s">
-        <v>363</v>
-      </c>
-      <c r="G7" s="71" t="s">
-        <v>592</v>
-      </c>
-      <c r="H7" s="75" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -10389,68 +10189,68 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="30">
-      <c r="A11" s="69" t="s">
-        <v>588</v>
+      <c r="A11" s="68" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>581</v>
+        <v>568</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>582</v>
+        <v>569</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="72" t="s">
-        <v>583</v>
+      <c r="A14" s="71" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>584</v>
+        <v>571</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="16" t="s">
-        <v>608</v>
+        <v>595</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="78" t="s">
-        <v>609</v>
+      <c r="A19" s="77" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="79" t="s">
-        <v>542</v>
+      <c r="A20" s="78" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="B22" s="59" t="s">
-        <v>605</v>
-      </c>
-      <c r="C22" s="59" t="s">
-        <v>610</v>
-      </c>
-      <c r="D22" s="59" t="s">
-        <v>611</v>
+      <c r="B22" s="58" t="s">
+        <v>592</v>
+      </c>
+      <c r="C22" s="58" t="s">
+        <v>597</v>
+      </c>
+      <c r="D22" s="58" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="68" t="s">
-        <v>604</v>
-      </c>
-      <c r="B23" s="68" t="s">
-        <v>601</v>
-      </c>
-      <c r="C23" s="68" t="s">
-        <v>602</v>
-      </c>
-      <c r="D23" s="68" t="s">
-        <v>603</v>
+      <c r="A23" s="67" t="s">
+        <v>591</v>
+      </c>
+      <c r="B23" s="67" t="s">
+        <v>588</v>
+      </c>
+      <c r="C23" s="67" t="s">
+        <v>589</v>
+      </c>
+      <c r="D23" s="67" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -10502,36 +10302,36 @@
         <v>377</v>
       </c>
       <c r="B1" s="46" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>526</v>
+        <v>513</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>527</v>
+        <v>514</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
       <c r="G1" s="46" t="s">
-        <v>529</v>
+        <v>516</v>
       </c>
       <c r="H1" s="46" t="s">
-        <v>530</v>
+        <v>517</v>
       </c>
       <c r="I1" s="46" t="s">
-        <v>531</v>
+        <v>518</v>
       </c>
       <c r="J1" s="46" t="s">
-        <v>532</v>
+        <v>519</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>533</v>
+        <v>520</v>
       </c>
       <c r="B2" s="37">
         <v>36526</v>
@@ -10555,15 +10355,15 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>534</v>
+        <v>521</v>
       </c>
       <c r="J2" t="s">
-        <v>535</v>
+        <v>522</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>536</v>
+        <v>523</v>
       </c>
       <c r="B3" s="37">
         <v>36526</v>
@@ -10587,10 +10387,10 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>537</v>
+        <v>524</v>
       </c>
       <c r="J3" t="s">
-        <v>538</v>
+        <v>525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pust 3/27 br 16
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/Bball SQL.xlsx
+++ b/BballMVC/_Documentation/Bball SQL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45C0E65-E75C-46F8-9920-08B61E384162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D570FD3-74F0-4E53-8FE8-6EBF820EF9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27750" yWindow="690" windowWidth="25200" windowHeight="14400" tabRatio="831" activeTab="3" xr2:uid="{3CF9E211-50E1-4178-837C-51B36022A708}"/>
+    <workbookView xWindow="27195" yWindow="660" windowWidth="25200" windowHeight="14400" tabRatio="831" activeTab="3" xr2:uid="{3CF9E211-50E1-4178-837C-51B36022A708}"/>
   </bookViews>
   <sheets>
     <sheet name="SPs" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">'Migrate DB'!$A$1:$E$95</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Parms!$A$1:$H$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'U Lg Parms'!$B$1:$AL$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">uspCalcTodaysMatchups!$A$1:$K$119</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">uspCalcTodaysMatchups!$A$1:$M$102</definedName>
     <definedName name="AverageAllowedOpPts">CalcGB4Pts!$B$20</definedName>
     <definedName name="AverageMadeUsPts">CalcGB4Pts!$B$19</definedName>
     <definedName name="BxScLinePct">'Curve %'!$C$2</definedName>
@@ -97,7 +97,7 @@
     <author>Keith</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{EE2F014B-DBE2-400B-A0C1-F919CB6A0134}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{EE2F014B-DBE2-400B-A0C1-F919CB6A0134}">
       <text>
         <r>
           <rPr>
@@ -111,7 +111,35 @@
         </r>
       </text>
     </comment>
-    <comment ref="G46" authorId="0" shapeId="0" xr:uid="{E87E8845-7127-490F-A019-21205554E175}">
+    <comment ref="E38" authorId="0" shapeId="0" xr:uid="{2496C311-CD5B-4CD1-91AA-F321EFFFB4A9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rotation &amp; TodaysMatchups are to retrived OurTotalLine or default to Rotation.TotalLine</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E46" authorId="0" shapeId="0" xr:uid="{AEBF64B0-4DE0-462D-ABFB-695BF2D72612}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rotation for Lines, TmStr for TmStrPtsOpp Scored / Allowed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I46" authorId="0" shapeId="0" xr:uid="{E87E8845-7127-490F-A019-21205554E175}">
       <text>
         <r>
           <rPr>
@@ -213,7 +241,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="752">
   <si>
     <t>Name</t>
   </si>
@@ -2643,16 +2671,10 @@
     <t>uspCalcTM3InsertTeamStatsAveragesRows - 22 Parms</t>
   </si>
   <si>
-    <t>uspQueryTM3TeamStatAveragesUnion - 19 Parms</t>
-  </si>
-  <si>
     <t>3.3.1</t>
   </si>
   <si>
     <t>@GB1-3, Aw/Hm, 0/1, @TeamAway/@TeamHome</t>
-  </si>
-  <si>
-    <t>uspQueryTM3TeamStatAverages - 19 Parms</t>
   </si>
   <si>
     <t>INSERT INTO TeamStatsAverages - 28 columns</t>
@@ -3265,6 +3287,51 @@
   <si>
     <t xml:space="preserve">WNBA      </t>
   </si>
+  <si>
+    <t>SP /UDFs</t>
+  </si>
+  <si>
+    <t>Sec #</t>
+  </si>
+  <si>
+    <t>Decommissioned</t>
+  </si>
+  <si>
+    <t>BoxScores, Rotation &amp; TodaysMatchups</t>
+  </si>
+  <si>
+    <t>BoxScores, Rotation &amp; TeamStrength</t>
+  </si>
+  <si>
+    <t>uspCalcTM3InsertTeamStatsAveragesRows</t>
+  </si>
+  <si>
+    <t>uspCalcTM3TeamStatAveragesUnion - 19 Parms</t>
+  </si>
+  <si>
+    <r>
+      <t>uspCalcTM3TeamStatAverages</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Union</t>
+    </r>
+  </si>
+  <si>
+    <t>uspCalcTM3TeamStatAverages - 19 Parms</t>
+  </si>
+  <si>
+    <t>uspCalcTM3TeamStatAverages</t>
+  </si>
+  <si>
+    <t>BxSc, Rot, TmStr, L5Min</t>
+  </si>
 </sst>
 </file>
 
@@ -3273,7 +3340,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3437,6 +3504,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="13">
@@ -3734,7 +3808,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -4029,6 +4103,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4051,13 +4132,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>381649</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>133475</xdr:rowOff>
@@ -4095,13 +4176,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>295912</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>133523</xdr:rowOff>
@@ -4139,13 +4220,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>86418</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>95343</xdr:rowOff>
@@ -5126,10 +5207,10 @@
   <sheetData>
     <row r="1" spans="2:38" s="53" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="117" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="C1" s="117" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="D1" s="117" t="s">
         <v>294</v>
@@ -5138,52 +5219,52 @@
         <v>427</v>
       </c>
       <c r="F1" s="117" t="s">
+        <v>708</v>
+      </c>
+      <c r="G1" s="117" t="s">
+        <v>709</v>
+      </c>
+      <c r="H1" s="117" t="s">
         <v>710</v>
       </c>
-      <c r="G1" s="117" t="s">
+      <c r="I1" s="117" t="s">
         <v>711</v>
       </c>
-      <c r="H1" s="117" t="s">
+      <c r="J1" s="117" t="s">
         <v>712</v>
       </c>
-      <c r="I1" s="117" t="s">
+      <c r="K1" s="117" t="s">
         <v>713</v>
       </c>
-      <c r="J1" s="117" t="s">
+      <c r="L1" s="117" t="s">
         <v>714</v>
       </c>
-      <c r="K1" s="117" t="s">
+      <c r="M1" s="117" t="s">
         <v>715</v>
       </c>
-      <c r="L1" s="117" t="s">
+      <c r="N1" s="117" t="s">
         <v>716</v>
       </c>
-      <c r="M1" s="117" t="s">
+      <c r="O1" s="117" t="s">
         <v>717</v>
       </c>
-      <c r="N1" s="117" t="s">
+      <c r="P1" s="117" t="s">
         <v>718</v>
       </c>
-      <c r="O1" s="117" t="s">
+      <c r="Q1" s="117" t="s">
         <v>719</v>
       </c>
-      <c r="P1" s="117" t="s">
+      <c r="R1" s="117" t="s">
         <v>720</v>
       </c>
-      <c r="Q1" s="117" t="s">
+      <c r="S1" s="117" t="s">
         <v>721</v>
       </c>
-      <c r="R1" s="117" t="s">
+      <c r="T1" s="117" t="s">
         <v>722</v>
       </c>
-      <c r="S1" s="117" t="s">
+      <c r="U1" s="117" t="s">
         <v>723</v>
-      </c>
-      <c r="T1" s="117" t="s">
-        <v>724</v>
-      </c>
-      <c r="U1" s="117" t="s">
-        <v>725</v>
       </c>
       <c r="V1" s="117" t="s">
         <v>488</v>
@@ -5195,46 +5276,46 @@
         <v>490</v>
       </c>
       <c r="Y1" s="117" t="s">
+        <v>724</v>
+      </c>
+      <c r="Z1" s="117" t="s">
+        <v>725</v>
+      </c>
+      <c r="AA1" s="117" t="s">
         <v>726</v>
       </c>
-      <c r="Z1" s="117" t="s">
+      <c r="AB1" s="117" t="s">
         <v>727</v>
       </c>
-      <c r="AA1" s="117" t="s">
+      <c r="AC1" s="117" t="s">
         <v>728</v>
       </c>
-      <c r="AB1" s="117" t="s">
+      <c r="AD1" s="117" t="s">
         <v>729</v>
       </c>
-      <c r="AC1" s="117" t="s">
+      <c r="AE1" s="117" t="s">
         <v>730</v>
       </c>
-      <c r="AD1" s="117" t="s">
+      <c r="AF1" s="117" t="s">
         <v>731</v>
       </c>
-      <c r="AE1" s="117" t="s">
+      <c r="AG1" s="117" t="s">
         <v>732</v>
       </c>
-      <c r="AF1" s="117" t="s">
+      <c r="AH1" s="117" t="s">
         <v>733</v>
       </c>
-      <c r="AG1" s="117" t="s">
+      <c r="AI1" s="117" t="s">
         <v>734</v>
       </c>
-      <c r="AH1" s="117" t="s">
+      <c r="AJ1" s="117" t="s">
         <v>735</v>
       </c>
-      <c r="AI1" s="117" t="s">
+      <c r="AK1" s="117" t="s">
         <v>736</v>
       </c>
-      <c r="AJ1" s="117" t="s">
+      <c r="AL1" s="117" t="s">
         <v>737</v>
-      </c>
-      <c r="AK1" s="117" t="s">
-        <v>738</v>
-      </c>
-      <c r="AL1" s="117" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="2" spans="2:38" x14ac:dyDescent="0.25">
@@ -5242,10 +5323,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D2" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E2" s="35">
         <v>36526</v>
@@ -5355,10 +5436,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>738</v>
+      </c>
+      <c r="D3" t="s">
         <v>740</v>
-      </c>
-      <c r="D3" t="s">
-        <v>742</v>
       </c>
       <c r="E3" s="35">
         <v>36526</v>
@@ -5468,10 +5549,10 @@
         <v>4010</v>
       </c>
       <c r="C4" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D4" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E4" s="35">
         <v>43466</v>
@@ -5581,10 +5662,10 @@
         <v>4011</v>
       </c>
       <c r="C5" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D5" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E5" s="35">
         <v>43739</v>
@@ -5694,10 +5775,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D6" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E6" s="35">
         <v>44075</v>
@@ -5807,10 +5888,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D7" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E7" s="35">
         <v>44089</v>
@@ -5920,10 +6001,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D8" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E8" s="35">
         <v>44175</v>
@@ -6033,10 +6114,10 @@
         <v>1001</v>
       </c>
       <c r="C9" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D9" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E9" s="35">
         <v>44191</v>
@@ -6146,10 +6227,10 @@
         <v>3004</v>
       </c>
       <c r="C10" t="s">
+        <v>738</v>
+      </c>
+      <c r="D10" t="s">
         <v>740</v>
-      </c>
-      <c r="D10" t="s">
-        <v>742</v>
       </c>
       <c r="E10" s="35">
         <v>44317</v>
@@ -6259,10 +6340,10 @@
         <v>1003</v>
       </c>
       <c r="C11" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D11" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E11" s="35">
         <v>44197</v>
@@ -6372,10 +6453,10 @@
         <v>3006</v>
       </c>
       <c r="C12" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D12" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E12" s="35">
         <v>44470</v>
@@ -6485,10 +6566,10 @@
         <v>3005</v>
       </c>
       <c r="C13" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D13" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E13" s="35">
         <v>44475</v>
@@ -6598,10 +6679,10 @@
         <v>4005</v>
       </c>
       <c r="C14" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D14" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E14" s="35">
         <v>44490</v>
@@ -6711,10 +6792,10 @@
         <v>4007</v>
       </c>
       <c r="C15" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D15" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E15" s="35">
         <v>44505</v>
@@ -6824,10 +6905,10 @@
         <v>4008</v>
       </c>
       <c r="C16" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D16" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E16" s="35">
         <v>44510</v>
@@ -6937,10 +7018,10 @@
         <v>4009</v>
       </c>
       <c r="C17" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D17" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E17" s="35">
         <v>44516</v>
@@ -7483,12 +7564,12 @@
     </row>
     <row r="19" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="20" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="22" spans="5:10" x14ac:dyDescent="0.25">
@@ -7556,7 +7637,7 @@
         <v>427</v>
       </c>
       <c r="F26" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="27" spans="5:10" x14ac:dyDescent="0.25">
@@ -11169,36 +11250,36 @@
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="44"/>
       <c r="B1" s="44" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="D1" s="44" t="s">
+        <v>686</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>691</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>692</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>688</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>692</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>693</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>694</v>
-      </c>
-      <c r="H1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>689</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>690</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="I2" s="114" t="s">
         <v>250</v>
@@ -11206,7 +11287,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="I3" s="114" t="s">
         <v>250</v>
@@ -11214,7 +11295,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="I4" s="114" t="s">
         <v>250</v>
@@ -11222,7 +11303,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="F5" s="114" t="s">
         <v>250</v>
@@ -11230,7 +11311,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="H6" s="114" t="s">
         <v>250</v>
@@ -11238,12 +11319,12 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="J8" s="114" t="s">
         <v>250</v>
@@ -11251,12 +11332,12 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="H10" s="114" t="s">
         <v>250</v>
@@ -11264,7 +11345,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="H11" s="114" t="s">
         <v>250</v>
@@ -11272,7 +11353,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="H12" s="114" t="s">
         <v>250</v>
@@ -11280,7 +11361,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="E13" s="114" t="s">
         <v>250</v>
@@ -11291,10 +11372,10 @@
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="D14" s="3" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="E14" s="114" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="F14" s="114" t="s">
         <v>250</v>
@@ -11302,10 +11383,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E15" s="114" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="F15" s="114" t="s">
         <v>250</v>
@@ -11313,10 +11394,10 @@
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="D16" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="E16" s="114" t="s">
         <v>697</v>
-      </c>
-      <c r="E16" s="114" t="s">
-        <v>699</v>
       </c>
       <c r="F16" s="114" t="s">
         <v>250</v>
@@ -11324,10 +11405,10 @@
     </row>
     <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D17" s="3" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="E17" s="114" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="F17" s="114" t="s">
         <v>250</v>
@@ -11335,13 +11416,13 @@
     </row>
     <row r="18" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C18" t="s">
+        <v>700</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>702</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>704</v>
       </c>
     </row>
   </sheetData>
@@ -11353,1521 +11434,1902 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0274D91-97AE-4EB7-A37C-618C93529D3A}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:X123"/>
+  <dimension ref="A1:Z123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38:XFD38"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="74.85546875" customWidth="1"/>
-    <col min="3" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" style="41" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
-    <col min="23" max="23" width="13.42578125" customWidth="1"/>
-    <col min="24" max="24" width="29.28515625" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="74.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="22.28515625" style="41" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="25" max="25" width="13.42578125" customWidth="1"/>
+    <col min="26" max="26" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="53" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="53" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="51" t="s">
+        <v>742</v>
+      </c>
+      <c r="B1" s="51" t="s">
         <v>414</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="C1" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="D1" s="51" t="s">
+        <v>741</v>
+      </c>
+      <c r="E1" s="51" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="F1" s="51" t="s">
+        <v>589</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" s="51" t="s">
+        <v>594</v>
+      </c>
+      <c r="I1" s="51" t="s">
+        <v>361</v>
+      </c>
+      <c r="J1" s="51" t="s">
+        <v>367</v>
+      </c>
+      <c r="K1" s="51" t="s">
+        <v>262</v>
+      </c>
+      <c r="L1" s="52" t="s">
+        <v>263</v>
+      </c>
+      <c r="M1" s="53" t="str">
+        <f>"SELECT  max(GameDate) as " &amp; G1 &amp; "MaxDate FROM " &amp; G1</f>
+        <v>SELECT  max(GameDate) as Table OutMaxDate FROM Table Out</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="48">
+        <v>1</v>
+      </c>
+      <c r="B2" s="48">
+        <v>1</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>519</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="H4" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>586</v>
+      </c>
+      <c r="C5" t="s">
+        <v>385</v>
+      </c>
+      <c r="E5" t="s">
+        <v>228</v>
+      </c>
+      <c r="H5" s="30"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1.2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>157</v>
+      </c>
+      <c r="H6" s="30"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1.3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1.4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>277</v>
+      </c>
+      <c r="E8" s="112" t="s">
+        <v>241</v>
+      </c>
+      <c r="F8" s="112"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="109" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="109" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="109" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="109" t="s">
+        <v>107</v>
+      </c>
+      <c r="W10" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="109" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" s="109" t="s">
+        <v>108</v>
+      </c>
+      <c r="W11" t="s">
+        <v>159</v>
+      </c>
+      <c r="X11" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="110" t="s">
+        <v>497</v>
+      </c>
+      <c r="F12" s="110" t="s">
+        <v>497</v>
+      </c>
+      <c r="I12">
+        <v>0.2</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="110" t="s">
+        <v>498</v>
+      </c>
+      <c r="F13" s="110" t="s">
+        <v>498</v>
+      </c>
+      <c r="I13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="110" t="s">
+        <v>499</v>
+      </c>
+      <c r="F14" s="110" t="s">
+        <v>499</v>
+      </c>
+      <c r="I14">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="109" t="s">
+        <v>156</v>
+      </c>
+      <c r="F15" s="109" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="109" t="s">
+        <v>442</v>
+      </c>
+      <c r="F16" s="109" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="111" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="111" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="111" t="s">
+        <v>156</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="111" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="111" t="s">
+        <v>391</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="111" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>596</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="I20" t="s">
+        <v>367</v>
+      </c>
+      <c r="J20" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" s="27">
+        <v>1.5</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>588</v>
+      </c>
+      <c r="E21" t="s">
+        <v>147</v>
+      </c>
+      <c r="H21" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" s="27"/>
+      <c r="C22" s="113" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="113" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>1.6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="F25" s="36" t="s">
         <v>591</v>
       </c>
-      <c r="E1" s="51" t="s">
-        <v>145</v>
-      </c>
-      <c r="F1" s="51" t="s">
-        <v>596</v>
-      </c>
-      <c r="G1" s="51" t="s">
-        <v>361</v>
-      </c>
-      <c r="H1" s="51" t="s">
-        <v>367</v>
-      </c>
-      <c r="I1" s="51" t="s">
-        <v>262</v>
-      </c>
-      <c r="J1" s="52" t="s">
-        <v>263</v>
-      </c>
-      <c r="K1" s="53" t="str">
-        <f>"SELECT  max(GameDate) as " &amp; E1 &amp; "MaxDate FROM " &amp; E1</f>
-        <v>SELECT  max(GameDate) as Table OutMaxDate FROM Table Out</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="48">
-        <v>1</v>
-      </c>
-      <c r="B2" s="48" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="14" t="s">
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>1.7</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>1.8</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>592</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>276</v>
+      </c>
+      <c r="F27" s="30"/>
+      <c r="G27" t="s">
+        <v>278</v>
+      </c>
+      <c r="H27" t="s">
+        <v>593</v>
+      </c>
+      <c r="I27" s="30"/>
+      <c r="L27" s="41" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>1.9</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="14"/>
+      <c r="E28" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="F28" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="G28" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B4" s="30" t="s">
-        <v>519</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="46" t="s">
-        <v>149</v>
-      </c>
-      <c r="F4" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
-        <v>588</v>
-      </c>
-      <c r="B5" t="s">
-        <v>385</v>
-      </c>
-      <c r="C5" t="s">
-        <v>228</v>
-      </c>
-      <c r="F5" s="30"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1.2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>157</v>
-      </c>
-      <c r="F6" s="30"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1.3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1.4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>277</v>
-      </c>
-      <c r="C8" s="112" t="s">
-        <v>241</v>
-      </c>
-      <c r="D8" s="112"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B9" s="109" t="s">
-        <v>106</v>
-      </c>
-      <c r="D9" s="109" t="s">
-        <v>106</v>
-      </c>
-      <c r="W9" t="s">
-        <v>163</v>
-      </c>
-      <c r="X9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B10" s="109" t="s">
-        <v>107</v>
-      </c>
-      <c r="D10" s="109" t="s">
-        <v>107</v>
-      </c>
-      <c r="U10" t="s">
-        <v>160</v>
-      </c>
-      <c r="W10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B11" s="109" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="109" t="s">
-        <v>108</v>
-      </c>
-      <c r="U11" t="s">
-        <v>159</v>
-      </c>
-      <c r="V11" t="s">
-        <v>161</v>
-      </c>
-      <c r="W11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B12" s="110" t="s">
-        <v>497</v>
-      </c>
-      <c r="D12" s="110" t="s">
-        <v>497</v>
-      </c>
-      <c r="G12">
-        <v>0.2</v>
-      </c>
-      <c r="W12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B13" s="110" t="s">
-        <v>498</v>
-      </c>
-      <c r="D13" s="110" t="s">
-        <v>498</v>
-      </c>
-      <c r="G13">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B14" s="110" t="s">
-        <v>499</v>
-      </c>
-      <c r="D14" s="110" t="s">
-        <v>499</v>
-      </c>
-      <c r="G14">
-        <v>0.67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B15" s="109" t="s">
-        <v>156</v>
-      </c>
-      <c r="D15" s="109" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B16" s="109" t="s">
-        <v>442</v>
-      </c>
-      <c r="D16" s="109" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="111" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="111" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="111" t="s">
-        <v>156</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="111" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="111" t="s">
-        <v>391</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="111" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
-        <v>598</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>589</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>592</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>597</v>
-      </c>
-      <c r="G20" t="s">
-        <v>367</v>
-      </c>
-      <c r="H20" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="27">
-        <v>1.5</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>590</v>
-      </c>
-      <c r="C21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="113" t="s">
-        <v>109</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
-      <c r="B23" s="113" t="s">
-        <v>110</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>1.6</v>
-      </c>
-      <c r="B24" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="28" t="s">
-        <v>275</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>225</v>
-      </c>
-      <c r="D25" s="36" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>1.7</v>
-      </c>
-      <c r="B26" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>1.8</v>
-      </c>
-      <c r="B27" s="30" t="s">
-        <v>594</v>
-      </c>
-      <c r="C27" s="30" t="s">
-        <v>276</v>
-      </c>
-      <c r="D27" s="30"/>
-      <c r="E27" t="s">
-        <v>278</v>
-      </c>
-      <c r="F27" t="s">
-        <v>595</v>
-      </c>
-      <c r="G27" s="30"/>
-      <c r="J27" s="41" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1.9</v>
-      </c>
-      <c r="B28" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="D28" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F28" s="30"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
+      <c r="H28" s="30"/>
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="13" t="s">
+      <c r="D29" s="13"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="F29" s="30"/>
-      <c r="G29" s="13" t="s">
+      <c r="H29" s="30"/>
+      <c r="I29" s="13" t="s">
         <v>367</v>
       </c>
-      <c r="H29" s="13" t="s">
+      <c r="J29" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="I29" s="13"/>
-      <c r="J29" s="45"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
+      <c r="K29" s="13"/>
+      <c r="L29" s="45"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
-      <c r="J30" s="45"/>
-      <c r="M30" t="s">
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="45"/>
+      <c r="O30" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="28" t="s">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="C31" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="G31" t="s">
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="I31" t="s">
         <v>367</v>
       </c>
-      <c r="H31" t="s">
+      <c r="J31" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="28" t="s">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="G32" t="s">
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="I32" t="s">
         <v>367</v>
       </c>
-      <c r="H32" t="s">
+      <c r="J32" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="29">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B33" s="36" t="s">
+      <c r="C33" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="J33" s="41" t="s">
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="L33" s="41" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="28" t="s">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="C34" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="37">
+    <row r="36" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" s="37">
         <v>1.1100000000000001</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="G36" t="s">
+      <c r="I36" t="s">
         <v>367</v>
       </c>
-      <c r="H36" t="s">
+      <c r="J36" t="s">
         <v>390</v>
       </c>
-      <c r="J36" s="41" t="s">
+      <c r="L36" s="41" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
         <v>1.1100000000000001</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="C37" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="14" t="s">
+      <c r="D37" s="14"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="F37" s="14"/>
-      <c r="G37" t="s">
+      <c r="H37" s="14"/>
+      <c r="I37" t="s">
         <v>427</v>
       </c>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
       <c r="J37" s="14"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="31" t="s">
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" s="31" t="s">
         <v>509</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" t="s">
+      <c r="D38" s="122" t="s">
+        <v>187</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>744</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="G38" t="s">
         <v>105</v>
       </c>
-      <c r="F38" t="s">
+      <c r="H38" t="s">
+        <v>593</v>
+      </c>
+      <c r="I38" s="30"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" s="31" t="s">
+        <v>510</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E39" t="s">
+        <v>105</v>
+      </c>
+      <c r="H39" s="30" t="s">
         <v>595</v>
       </c>
-      <c r="G38" s="30"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
-        <v>510</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C39" t="s">
-        <v>105</v>
-      </c>
-      <c r="F39" s="30" t="s">
-        <v>597</v>
-      </c>
-      <c r="G39" t="s">
+      <c r="I39" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="31" t="s">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40" s="31" t="s">
         <v>515</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="F40" s="30"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H40" s="30"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="48">
         <v>2</v>
       </c>
-      <c r="B41" s="49"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="G41" t="s">
+      <c r="B41" s="48">
+        <v>2</v>
+      </c>
+      <c r="C41" s="49"/>
+      <c r="D41" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="I41" t="s">
         <v>274</v>
       </c>
-      <c r="H41" t="s">
+      <c r="J41" t="s">
         <v>392</v>
       </c>
-      <c r="I41" s="13" t="s">
+      <c r="K41" s="13" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="2" t="s">
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>2</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="2" t="s">
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>2</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="I44" t="s">
+      <c r="D44" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="5" t="s">
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="K44" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="D45" s="14"/>
+      <c r="E45" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="D45" s="5"/>
-      <c r="E45" s="14" t="s">
+      <c r="F45" s="5"/>
+      <c r="G45" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
       <c r="H45" s="14"/>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="5" t="s">
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" t="s">
+      <c r="D46" s="122" t="s">
+        <v>193</v>
+      </c>
+      <c r="E46" s="30" t="s">
+        <v>745</v>
+      </c>
+      <c r="F46" s="5"/>
+      <c r="G46" t="s">
         <v>42</v>
       </c>
-      <c r="G46" t="s">
+      <c r="I46" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="5" t="s">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="G47" t="s">
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="I47" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="5" t="s">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="48">
         <v>3</v>
       </c>
-      <c r="B49" s="50" t="s">
+      <c r="B49" s="48">
+        <v>3</v>
+      </c>
+      <c r="C49" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="48">
+      <c r="E49" s="30"/>
+      <c r="F49" s="30"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50" s="48">
         <v>3.1</v>
       </c>
-      <c r="B50" s="99" t="s">
+      <c r="C50" s="99" t="s">
         <v>560</v>
       </c>
-      <c r="C50" s="30">
+      <c r="D50" s="124" t="s">
+        <v>746</v>
+      </c>
+      <c r="E50" s="30">
         <v>22</v>
       </c>
-      <c r="D50" s="30"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="48">
+      <c r="F50" s="30"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51" s="48">
         <v>3.1</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="C51" s="30"/>
-      <c r="D51" s="30"/>
-      <c r="E51">
+      <c r="C51" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="E51" s="30"/>
+      <c r="F51" s="30"/>
+      <c r="G51">
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="48">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="B52" s="48">
         <v>3.2</v>
       </c>
-      <c r="B52" s="98" t="s">
+      <c r="C52" s="98" t="s">
+        <v>747</v>
+      </c>
+      <c r="D52" s="123" t="s">
+        <v>748</v>
+      </c>
+      <c r="E52" s="30">
+        <v>19</v>
+      </c>
+      <c r="F52" s="30"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>3</v>
+      </c>
+      <c r="B53" s="48">
+        <v>3.2</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E53" s="30"/>
+      <c r="F53" s="30"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>3</v>
+      </c>
+      <c r="B54" s="48">
+        <v>3.2</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="E54" s="30"/>
+      <c r="F54" s="30"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>3</v>
+      </c>
+      <c r="B55" s="48">
+        <v>3.3</v>
+      </c>
+      <c r="C55" s="101" t="s">
+        <v>749</v>
+      </c>
+      <c r="D55" s="123" t="s">
+        <v>750</v>
+      </c>
+      <c r="E55" s="30" t="s">
+        <v>751</v>
+      </c>
+      <c r="F55" s="30"/>
+      <c r="G55">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>3</v>
+      </c>
+      <c r="B56" s="48" t="s">
         <v>561</v>
       </c>
-      <c r="C52" s="30">
-        <v>19</v>
-      </c>
-      <c r="D52" s="30"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="48">
+      <c r="C56" s="100" t="s">
+        <v>562</v>
+      </c>
+      <c r="E56" s="30"/>
+      <c r="F56" s="30"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>3</v>
+      </c>
+      <c r="B57">
+        <v>3.1</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>3</v>
+      </c>
+      <c r="B58">
         <v>3.2</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C58" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>3</v>
+      </c>
+      <c r="B59" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="48">
-        <v>3.2</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>559</v>
-      </c>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="48">
-        <v>3.3</v>
-      </c>
-      <c r="B55" s="101" t="s">
-        <v>564</v>
-      </c>
-      <c r="C55" s="30">
-        <v>19</v>
-      </c>
-      <c r="D55" s="30"/>
-      <c r="E55">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="48" t="s">
-        <v>562</v>
-      </c>
-      <c r="B56" s="100" t="s">
-        <v>563</v>
-      </c>
-      <c r="C56" s="30"/>
-      <c r="D56" s="30"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>3.1</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>3.2</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="31" t="s">
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>3</v>
+      </c>
+      <c r="B60" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="C60" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="31" t="s">
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>3</v>
+      </c>
+      <c r="B61" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="B61" s="32" t="s">
+      <c r="C61" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="C61" s="32"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="14" t="s">
+      <c r="D61" s="14"/>
+      <c r="E61" s="32"/>
+      <c r="F61" s="32"/>
+      <c r="G61" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="F61" s="14"/>
-      <c r="G61" s="14"/>
       <c r="H61" s="14"/>
       <c r="I61" s="14"/>
       <c r="J61" s="14"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B62" s="33" t="s">
+      <c r="K61" s="14"/>
+      <c r="L61" s="14"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>3</v>
+      </c>
+      <c r="C62" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="C62" s="33"/>
-      <c r="D62" s="33"/>
-      <c r="E62" t="s">
+      <c r="E62" s="33"/>
+      <c r="F62" s="33"/>
+      <c r="G62" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B63" s="33" t="s">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>3</v>
+      </c>
+      <c r="C63" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="C63" s="33"/>
-      <c r="D63" s="33"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B64" s="34" t="s">
+      <c r="E63" s="33"/>
+      <c r="F63" s="33"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>3</v>
+      </c>
+      <c r="C64" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="C64" s="34"/>
-      <c r="D64" s="34"/>
-      <c r="K64" t="s">
+      <c r="E64" s="34"/>
+      <c r="F64" s="34"/>
+      <c r="M64" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B65" s="34" t="s">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>3</v>
+      </c>
+      <c r="C65" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="C65" s="34"/>
-      <c r="D65" s="34"/>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B66" s="33" t="s">
+      <c r="E65" s="34"/>
+      <c r="F65" s="34"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>3</v>
+      </c>
+      <c r="C66" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="C66" s="33"/>
-      <c r="D66" s="33"/>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B67" s="34" t="s">
+      <c r="E66" s="33"/>
+      <c r="F66" s="33"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>3</v>
+      </c>
+      <c r="C67" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="C67" s="33"/>
-      <c r="D67" s="33"/>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E67" s="33"/>
+      <c r="F67" s="33"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="48">
         <v>4</v>
       </c>
-      <c r="B68" s="50" t="s">
+      <c r="B68" s="48">
+        <v>4</v>
+      </c>
+      <c r="C68" s="50" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69">
+        <v>4</v>
+      </c>
+      <c r="B69">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70">
+        <v>4</v>
+      </c>
+      <c r="B70">
         <v>4.2</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>153</v>
       </c>
-      <c r="M70">
+      <c r="O70">
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71">
+        <v>4</v>
+      </c>
+      <c r="B71">
         <v>4.3</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
         <v>154</v>
       </c>
-      <c r="M71">
+      <c r="O71">
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A72" s="31">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>4</v>
+      </c>
+      <c r="B72" s="31">
         <v>4.3099999999999996</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
         <v>155</v>
       </c>
-      <c r="M72">
+      <c r="O72">
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>4</v>
+      </c>
+      <c r="C73" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B74" s="4" t="s">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>4</v>
+      </c>
+      <c r="C74" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
-    </row>
-    <row r="75" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="26" t="s">
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
+    </row>
+    <row r="75" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>4</v>
+      </c>
+      <c r="C75" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C75" s="26"/>
-      <c r="D75" s="26"/>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E75" s="26"/>
+      <c r="F75" s="26"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76">
+        <v>4</v>
+      </c>
+      <c r="B76">
         <v>4.32</v>
       </c>
-      <c r="B76" s="26" t="s">
+      <c r="C76" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="C76" s="26"/>
-      <c r="D76" s="26"/>
-    </row>
-    <row r="77" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="26" t="s">
+      <c r="E76" s="26"/>
+      <c r="F76" s="26"/>
+    </row>
+    <row r="77" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>4</v>
+      </c>
+      <c r="C77" s="26" t="s">
         <v>266</v>
       </c>
-      <c r="C77" s="26"/>
-      <c r="D77" s="26"/>
-      <c r="I77" t="s">
+      <c r="D77" t="s">
         <v>267</v>
       </c>
-      <c r="J77" s="41" t="s">
+      <c r="E77" s="26"/>
+      <c r="F77" s="26"/>
+      <c r="K77" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L77" s="41" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78">
+        <v>4</v>
+      </c>
+      <c r="B78">
         <v>4.33</v>
       </c>
-      <c r="B78" s="26" t="s">
+      <c r="C78" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="C78" s="26"/>
-      <c r="D78" s="26"/>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E78" s="26"/>
+      <c r="F78" s="26"/>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79">
+        <v>4</v>
+      </c>
+      <c r="B79">
         <v>4.3499999999999996</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="14" t="s">
+      <c r="D79" s="14"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="F79" s="14"/>
-      <c r="G79" s="14"/>
       <c r="H79" s="14"/>
       <c r="I79" s="14"/>
       <c r="J79" s="14"/>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K79" s="14"/>
+      <c r="L79" s="14"/>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80">
+        <v>4</v>
+      </c>
+      <c r="B80">
         <v>4.3499999999999996</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="14"/>
-      <c r="F80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
       <c r="G80" s="14"/>
       <c r="H80" s="14"/>
       <c r="I80" s="14"/>
       <c r="J80" s="14"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B81" s="58" t="s">
+      <c r="K80" s="14"/>
+      <c r="L80" s="14"/>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>4</v>
+      </c>
+      <c r="C81" s="58" t="s">
         <v>478</v>
       </c>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="14"/>
-      <c r="F81" s="14"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
       <c r="G81" s="14"/>
       <c r="H81" s="14"/>
       <c r="I81" s="14"/>
       <c r="J81" s="14"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B82" s="58" t="s">
+      <c r="K81" s="14"/>
+      <c r="L81" s="14"/>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>4</v>
+      </c>
+      <c r="C82" s="58" t="s">
         <v>479</v>
       </c>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="14"/>
-      <c r="F82" s="14"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
       <c r="G82" s="14"/>
       <c r="H82" s="14"/>
       <c r="I82" s="14"/>
       <c r="J82" s="14"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B83" s="58" t="s">
+      <c r="K82" s="14"/>
+      <c r="L82" s="14"/>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>4</v>
+      </c>
+      <c r="C83" s="58" t="s">
         <v>480</v>
       </c>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="14"/>
-      <c r="F83" s="14"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
       <c r="G83" s="14"/>
       <c r="H83" s="14"/>
       <c r="I83" s="14"/>
       <c r="J83" s="14"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K83" s="14"/>
+      <c r="L83" s="14"/>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84">
+        <v>4</v>
+      </c>
+      <c r="B84">
         <v>4.3499999999999996</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="14"/>
+      <c r="D84" s="14"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
       <c r="G84" s="14"/>
       <c r="H84" s="14"/>
       <c r="I84" s="14"/>
       <c r="J84" s="14"/>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B85" s="62" t="s">
+      <c r="K84" s="14"/>
+      <c r="L84" s="14"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>4</v>
+      </c>
+      <c r="C85" s="62" t="s">
         <v>459</v>
       </c>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="14"/>
-      <c r="F85" s="14"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
       <c r="G85" s="14"/>
       <c r="H85" s="14"/>
       <c r="I85" s="14"/>
       <c r="J85" s="14"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B86" s="62" t="s">
+      <c r="K85" s="14"/>
+      <c r="L85" s="14"/>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>4</v>
+      </c>
+      <c r="C86" s="62" t="s">
         <v>460</v>
       </c>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="14"/>
-      <c r="F86" s="14"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
       <c r="G86" s="14"/>
       <c r="H86" s="14"/>
       <c r="I86" s="14"/>
       <c r="J86" s="14"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B87" s="62" t="s">
+      <c r="K86" s="14"/>
+      <c r="L86" s="14"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>4</v>
+      </c>
+      <c r="C87" s="62" t="s">
         <v>461</v>
       </c>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="14"/>
-      <c r="F87" s="14"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
       <c r="G87" s="14"/>
       <c r="H87" s="14"/>
       <c r="I87" s="14"/>
       <c r="J87" s="14"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B88" s="62" t="s">
+      <c r="K87" s="14"/>
+      <c r="L87" s="14"/>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>4</v>
+      </c>
+      <c r="C88" s="62" t="s">
         <v>462</v>
       </c>
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="14"/>
-      <c r="F88" s="14"/>
+      <c r="D88" s="14"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
       <c r="G88" s="14"/>
       <c r="H88" s="14"/>
       <c r="I88" s="14"/>
       <c r="J88" s="14"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B89" s="62" t="s">
+      <c r="K88" s="14"/>
+      <c r="L88" s="14"/>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>4</v>
+      </c>
+      <c r="C89" s="62" t="s">
         <v>463</v>
       </c>
-      <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="14"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
       <c r="G89" s="14"/>
       <c r="H89" s="14"/>
       <c r="I89" s="14"/>
       <c r="J89" s="14"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B90" s="62" t="s">
+      <c r="K89" s="14"/>
+      <c r="L89" s="14"/>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>4</v>
+      </c>
+      <c r="C90" s="62" t="s">
         <v>464</v>
       </c>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
-      <c r="E90" s="14"/>
-      <c r="F90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
       <c r="G90" s="14"/>
       <c r="H90" s="14"/>
       <c r="I90" s="14"/>
       <c r="J90" s="14"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B91" s="63" t="s">
+      <c r="K90" s="14"/>
+      <c r="L90" s="14"/>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>4</v>
+      </c>
+      <c r="C91" s="63" t="s">
         <v>465</v>
       </c>
-      <c r="C91" s="14"/>
-      <c r="D91" s="14"/>
       <c r="E91" s="14"/>
       <c r="F91" s="14"/>
       <c r="G91" s="14"/>
       <c r="H91" s="14"/>
-      <c r="J91"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B92" s="63" t="s">
+      <c r="I91" s="14"/>
+      <c r="J91" s="14"/>
+      <c r="L91"/>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>4</v>
+      </c>
+      <c r="C92" s="63" t="s">
         <v>466</v>
       </c>
-      <c r="C92" s="14" t="s">
+      <c r="E92" s="14" t="s">
         <v>467</v>
       </c>
-      <c r="D92" s="14"/>
-      <c r="E92" s="14"/>
       <c r="F92" s="14"/>
       <c r="G92" s="14"/>
       <c r="H92" s="14"/>
-      <c r="J92"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B93" s="63" t="s">
+      <c r="I92" s="14"/>
+      <c r="J92" s="14"/>
+      <c r="L92"/>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>4</v>
+      </c>
+      <c r="C93" s="63" t="s">
         <v>468</v>
       </c>
-      <c r="C93" s="14"/>
-      <c r="D93" s="14"/>
       <c r="E93" s="14"/>
       <c r="F93" s="14"/>
       <c r="G93" s="14"/>
       <c r="H93" s="14"/>
-      <c r="J93"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B94" s="62" t="s">
+      <c r="I93" s="14"/>
+      <c r="J93" s="14"/>
+      <c r="L93"/>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>4</v>
+      </c>
+      <c r="C94" s="62" t="s">
         <v>469</v>
       </c>
-      <c r="C94" s="14"/>
       <c r="D94" s="14"/>
       <c r="E94" s="14"/>
       <c r="F94" s="14"/>
       <c r="G94" s="14"/>
       <c r="H94" s="14"/>
       <c r="I94" s="14"/>
-      <c r="J94"/>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B95" s="62" t="s">
+      <c r="J94" s="14"/>
+      <c r="K94" s="14"/>
+      <c r="L94"/>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>4</v>
+      </c>
+      <c r="C95" s="62" t="s">
         <v>470</v>
       </c>
-      <c r="C95" s="1"/>
-      <c r="D95" s="1"/>
-      <c r="E95" s="14"/>
-      <c r="F95" s="14"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
       <c r="G95" s="14"/>
       <c r="H95" s="14"/>
       <c r="I95" s="14"/>
       <c r="J95" s="14"/>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B96" s="63" t="s">
+      <c r="K95" s="14"/>
+      <c r="L95" s="14"/>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>4</v>
+      </c>
+      <c r="C96" s="63" t="s">
         <v>465</v>
       </c>
-      <c r="C96" s="14"/>
-      <c r="D96" s="14"/>
       <c r="E96" s="14"/>
       <c r="F96" s="14"/>
       <c r="G96" s="14"/>
       <c r="H96" s="14"/>
-      <c r="J96"/>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B97" s="63" t="s">
+      <c r="I96" s="14"/>
+      <c r="J96" s="14"/>
+      <c r="L96"/>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>4</v>
+      </c>
+      <c r="C97" s="63" t="s">
         <v>471</v>
       </c>
-      <c r="C97" s="14" t="s">
+      <c r="E97" s="14" t="s">
         <v>467</v>
       </c>
-      <c r="D97" s="14"/>
-      <c r="E97" s="14"/>
       <c r="F97" s="14"/>
       <c r="G97" s="14"/>
       <c r="H97" s="14"/>
-      <c r="J97"/>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B98" s="63" t="s">
+      <c r="I97" s="14"/>
+      <c r="J97" s="14"/>
+      <c r="L97"/>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>4</v>
+      </c>
+      <c r="C98" s="63" t="s">
         <v>472</v>
       </c>
-      <c r="C98" s="14"/>
-      <c r="D98" s="14"/>
       <c r="E98" s="14"/>
       <c r="F98" s="14"/>
       <c r="G98" s="14"/>
       <c r="H98" s="14"/>
-      <c r="J98"/>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B99" s="63" t="s">
+      <c r="I98" s="14"/>
+      <c r="J98" s="14"/>
+      <c r="L98"/>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>4</v>
+      </c>
+      <c r="C99" s="63" t="s">
         <v>473</v>
       </c>
-      <c r="C99" s="14"/>
-      <c r="D99" s="14"/>
       <c r="E99" s="14"/>
       <c r="F99" s="14"/>
       <c r="G99" s="14"/>
       <c r="H99" s="14"/>
-      <c r="J99"/>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B100" s="63" t="s">
+      <c r="I99" s="14"/>
+      <c r="J99" s="14"/>
+      <c r="L99"/>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>4</v>
+      </c>
+      <c r="C100" s="63" t="s">
         <v>474</v>
       </c>
-      <c r="C100" s="14"/>
-      <c r="D100" s="14"/>
       <c r="E100" s="14"/>
       <c r="F100" s="14"/>
       <c r="G100" s="14"/>
       <c r="H100" s="14"/>
-      <c r="J100"/>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B101" s="62" t="s">
+      <c r="I100" s="14"/>
+      <c r="J100" s="14"/>
+      <c r="L100"/>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>4</v>
+      </c>
+      <c r="C101" s="62" t="s">
         <v>475</v>
       </c>
-      <c r="E101" s="14"/>
-      <c r="F101" s="14"/>
+      <c r="D101" s="14"/>
       <c r="G101" s="14"/>
       <c r="H101" s="14"/>
       <c r="I101" s="14"/>
       <c r="J101" s="14"/>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B102" s="62" t="s">
+      <c r="K101" s="14"/>
+      <c r="L101" s="14"/>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>4</v>
+      </c>
+      <c r="C102" s="62" t="s">
         <v>476</v>
       </c>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
-      <c r="E102" s="14"/>
-      <c r="F102" s="14"/>
+      <c r="D102" s="14"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
       <c r="G102" s="14"/>
       <c r="H102" s="14"/>
       <c r="I102" s="14"/>
       <c r="J102" s="14"/>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B103" s="1"/>
+      <c r="K102" s="14"/>
+      <c r="L102" s="14"/>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
-      <c r="E103" s="14"/>
-      <c r="F103" s="14"/>
+      <c r="D103" s="14"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
       <c r="G103" s="14"/>
       <c r="H103" s="14"/>
       <c r="I103" s="14"/>
       <c r="J103" s="14"/>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B104" s="1"/>
+      <c r="K103" s="14"/>
+      <c r="L103" s="14"/>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-      <c r="E104" s="14"/>
-      <c r="F104" s="14"/>
+      <c r="D104" s="14"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
       <c r="G104" s="14"/>
       <c r="H104" s="14"/>
       <c r="I104" s="14"/>
       <c r="J104" s="14"/>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A105">
+      <c r="K104" s="14"/>
+      <c r="L104" s="14"/>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B105">
         <v>4.3499999999999996</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="C105" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
-      <c r="E105" s="14"/>
-      <c r="F105" s="14"/>
+      <c r="D105" s="14"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
       <c r="G105" s="14"/>
       <c r="H105" s="14"/>
       <c r="I105" s="14"/>
       <c r="J105" s="14"/>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B106" s="58" t="s">
+      <c r="K105" s="14"/>
+      <c r="L105" s="14"/>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C106" s="58" t="s">
         <v>448</v>
       </c>
-      <c r="C106" s="58"/>
-      <c r="D106" s="58"/>
-      <c r="E106" s="59"/>
-      <c r="F106" s="59"/>
+      <c r="D106" s="59"/>
+      <c r="E106" s="58"/>
+      <c r="F106" s="58"/>
       <c r="G106" s="59"/>
       <c r="H106" s="59"/>
       <c r="I106" s="59"/>
       <c r="J106" s="59"/>
-      <c r="K106" s="60"/>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B107" s="58" t="s">
+      <c r="K106" s="59"/>
+      <c r="L106" s="59"/>
+      <c r="M106" s="60"/>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C107" s="58" t="s">
         <v>456</v>
       </c>
-      <c r="E107" s="59"/>
-      <c r="F107" s="59"/>
+      <c r="D107" s="59"/>
       <c r="G107" s="59"/>
       <c r="H107" s="59"/>
       <c r="I107" s="59"/>
       <c r="J107" s="59"/>
-      <c r="K107" s="60"/>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B108" s="58" t="s">
+      <c r="K107" s="59"/>
+      <c r="L107" s="59"/>
+      <c r="M107" s="60"/>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C108" s="58" t="s">
         <v>449</v>
       </c>
-      <c r="C108" s="58"/>
-      <c r="D108" s="58"/>
-      <c r="E108" s="59"/>
-      <c r="F108" s="59"/>
+      <c r="D108" s="59"/>
+      <c r="E108" s="58"/>
+      <c r="F108" s="58"/>
       <c r="G108" s="59"/>
       <c r="H108" s="59"/>
       <c r="I108" s="59"/>
       <c r="J108" s="59"/>
-      <c r="K108" s="60"/>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B109" s="58" t="s">
+      <c r="K108" s="59"/>
+      <c r="L108" s="59"/>
+      <c r="M108" s="60"/>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C109" s="58" t="s">
         <v>450</v>
       </c>
-      <c r="C109" s="58"/>
-      <c r="D109" s="58"/>
-      <c r="E109" s="59"/>
-      <c r="F109" s="59"/>
+      <c r="D109" s="59"/>
+      <c r="E109" s="58"/>
+      <c r="F109" s="58"/>
       <c r="G109" s="59"/>
       <c r="H109" s="59"/>
       <c r="I109" s="59"/>
       <c r="J109" s="59"/>
-      <c r="K109" s="60"/>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B110" s="59" t="s">
+      <c r="K109" s="59"/>
+      <c r="L109" s="59"/>
+      <c r="M109" s="60"/>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C110" s="59" t="s">
         <v>451</v>
       </c>
-      <c r="C110" s="58"/>
-      <c r="D110" s="58"/>
-      <c r="G110" s="59"/>
-      <c r="H110" s="59"/>
+      <c r="D110" s="59"/>
+      <c r="E110" s="58"/>
+      <c r="F110" s="58"/>
       <c r="I110" s="59"/>
       <c r="J110" s="59"/>
-      <c r="K110" s="60" t="s">
+      <c r="K110" s="59"/>
+      <c r="L110" s="59"/>
+      <c r="M110" s="60" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B111" s="58" t="s">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C111" s="58" t="s">
         <v>453</v>
       </c>
-      <c r="C111" s="58"/>
-      <c r="D111" s="58"/>
-      <c r="E111" s="59"/>
-      <c r="F111" s="59"/>
+      <c r="D111" s="59"/>
+      <c r="E111" s="58"/>
+      <c r="F111" s="58"/>
       <c r="G111" s="59"/>
       <c r="H111" s="59"/>
       <c r="I111" s="59"/>
       <c r="J111" s="59"/>
-      <c r="K111" s="60"/>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B112" s="58" t="s">
+      <c r="K111" s="59"/>
+      <c r="L111" s="59"/>
+      <c r="M111" s="60"/>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C112" s="58" t="s">
         <v>454</v>
       </c>
-      <c r="C112" s="58"/>
-      <c r="D112" s="58"/>
-      <c r="E112" s="59"/>
-      <c r="F112" s="59"/>
+      <c r="D112" s="59"/>
+      <c r="E112" s="58"/>
+      <c r="F112" s="58"/>
       <c r="G112" s="59"/>
       <c r="H112" s="59"/>
       <c r="I112" s="59"/>
       <c r="J112" s="59"/>
-      <c r="K112" s="60"/>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B113" s="58" t="s">
+      <c r="K112" s="59"/>
+      <c r="L112" s="59"/>
+      <c r="M112" s="60"/>
+    </row>
+    <row r="113" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C113" s="58" t="s">
         <v>455</v>
       </c>
-      <c r="C113" s="58"/>
-      <c r="D113" s="58"/>
-      <c r="E113" s="59"/>
-      <c r="F113" s="59"/>
+      <c r="D113" s="59"/>
+      <c r="E113" s="58"/>
+      <c r="F113" s="58"/>
       <c r="G113" s="59"/>
-      <c r="H113" s="61" t="s">
+      <c r="H113" s="59"/>
+      <c r="I113" s="59"/>
+      <c r="J113" s="61" t="s">
         <v>457</v>
       </c>
-      <c r="I113" s="59"/>
-      <c r="J113" s="59"/>
-      <c r="K113" s="60"/>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A114">
+      <c r="K113" s="59"/>
+      <c r="L113" s="59"/>
+      <c r="M113" s="60"/>
+    </row>
+    <row r="114" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B114">
         <v>4.3499999999999996</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="C114" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="C114" s="1"/>
-      <c r="D114" s="1"/>
-      <c r="E114" s="14"/>
-      <c r="F114" s="14"/>
+      <c r="D114" s="14"/>
+      <c r="E114" s="1"/>
+      <c r="F114" s="1"/>
       <c r="G114" s="14"/>
       <c r="H114" s="14"/>
       <c r="I114" s="14"/>
       <c r="J114" s="14"/>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B115" s="57" t="s">
+      <c r="K114" s="14"/>
+      <c r="L114" s="14"/>
+    </row>
+    <row r="115" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C115" s="57" t="s">
         <v>444</v>
       </c>
-      <c r="C115" s="1"/>
-      <c r="D115" s="1"/>
-      <c r="E115" s="14"/>
-      <c r="F115" s="14"/>
+      <c r="D115" s="14"/>
+      <c r="E115" s="1"/>
+      <c r="F115" s="1"/>
       <c r="G115" s="14"/>
       <c r="H115" s="14"/>
       <c r="I115" s="14"/>
       <c r="J115" s="14"/>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B116" s="64" t="s">
+      <c r="K115" s="14"/>
+      <c r="L115" s="14"/>
+    </row>
+    <row r="116" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C116" s="64" t="s">
         <v>445</v>
       </c>
-      <c r="C116" s="1"/>
-      <c r="D116" s="1"/>
-      <c r="E116" s="14"/>
-      <c r="F116" s="14"/>
+      <c r="D116" s="14"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
       <c r="G116" s="14"/>
       <c r="H116" s="14"/>
       <c r="I116" s="14"/>
       <c r="J116" s="14"/>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B117" s="57" t="s">
+      <c r="K116" s="14"/>
+      <c r="L116" s="14"/>
+    </row>
+    <row r="117" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C117" s="57" t="s">
         <v>446</v>
       </c>
-      <c r="C117" s="1"/>
-      <c r="D117" s="1"/>
-      <c r="E117" s="14"/>
-      <c r="F117" s="14"/>
+      <c r="D117" s="14"/>
+      <c r="E117" s="1"/>
+      <c r="F117" s="1"/>
       <c r="G117" s="14"/>
       <c r="H117" s="14"/>
       <c r="I117" s="14"/>
       <c r="J117" s="14"/>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B118" s="1"/>
+      <c r="K117" s="14"/>
+      <c r="L117" s="14"/>
+    </row>
+    <row r="118" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C118" s="1"/>
-      <c r="D118" s="1"/>
-      <c r="E118" s="14"/>
-      <c r="F118" s="14"/>
+      <c r="D118" s="14"/>
+      <c r="E118" s="1"/>
+      <c r="F118" s="1"/>
       <c r="G118" s="14"/>
       <c r="H118" s="14"/>
       <c r="I118" s="14"/>
       <c r="J118" s="14"/>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B119" s="2" t="s">
+      <c r="K118" s="14"/>
+      <c r="L118" s="14"/>
+    </row>
+    <row r="119" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C119" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C119" s="2"/>
-      <c r="D119" s="2"/>
-      <c r="E119" t="s">
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
+      <c r="G119" t="s">
         <v>40</v>
       </c>
-      <c r="K119" t="str">
-        <f>"SELECT  max(GameDate) as MaxDate FROM " &amp; E119</f>
+      <c r="M119" t="str">
+        <f>"SELECT  max(GameDate) as MaxDate FROM " &amp; G119</f>
         <v>SELECT  max(GameDate) as MaxDate FROM TodaysMatchups</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B120" s="2"/>
+    <row r="120" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C120" s="2"/>
-      <c r="D120" s="2"/>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B122" s="1" t="s">
+      <c r="E120" s="2"/>
+      <c r="F120" s="2"/>
+    </row>
+    <row r="122" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C122" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C122" s="14" t="s">
+      <c r="E122" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D122" s="14"/>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B123" s="30" t="s">
+      <c r="F122" s="14"/>
+    </row>
+    <row r="123" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C123" s="30" t="s">
         <v>254</v>
       </c>
-      <c r="C123" t="s">
+      <c r="E123" t="s">
         <v>252</v>
       </c>
-      <c r="E123" t="s">
+      <c r="G123" t="s">
         <v>149</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K119" xr:uid="{A7814D99-45DC-4222-B9C2-8A06FBE29E7B}"/>
+  <autoFilter ref="A1:M102" xr:uid="{B0274D91-97AE-4EB7-A37C-618C93529D3A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -12896,7 +13358,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="115" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B1" s="115" t="s">
         <v>348</v>
@@ -12914,18 +13376,18 @@
         <v>4</v>
       </c>
       <c r="G1" s="115" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="H1" s="115" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B2" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="D2" t="s">
         <v>250</v>
@@ -12934,15 +13396,15 @@
         <v>250</v>
       </c>
       <c r="G2" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B3" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="D3" t="s">
         <v>250</v>
@@ -12951,143 +13413,143 @@
         <v>250</v>
       </c>
       <c r="G3" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B4" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B5" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B6" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B7" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B8" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B9" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B10" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B11" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B12" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B13" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B14" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B15" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B16" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B17" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B18" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B19" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B20" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="G20" t="s">
         <v>509</v>
@@ -13098,52 +13560,52 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B21" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="E21" t="s">
         <v>250</v>
       </c>
       <c r="G21" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B22" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="E22" t="s">
         <v>250</v>
       </c>
       <c r="G22" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B23" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="E23" t="s">
         <v>250</v>
       </c>
       <c r="G23" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B24" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="F24" t="s">
         <v>250</v>
@@ -13154,10 +13616,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B25" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="F25" t="s">
         <v>250</v>
@@ -13168,10 +13630,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B26" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="F26" t="s">
         <v>250</v>
@@ -13182,10 +13644,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B27" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="F27" t="s">
         <v>250</v>
@@ -13196,10 +13658,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="99" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B28" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="C28" t="s">
         <v>272</v>
@@ -13214,15 +13676,15 @@
         <v>250</v>
       </c>
       <c r="G28" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="99" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B29" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="C29" t="s">
         <v>272</v>
@@ -13231,15 +13693,15 @@
         <v>250</v>
       </c>
       <c r="G29" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="99" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B30" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="C30" t="s">
         <v>272</v>
@@ -13251,32 +13713,32 @@
         <v>250</v>
       </c>
       <c r="G30" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="H30" s="41" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B31" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="E31" t="s">
         <v>250</v>
       </c>
       <c r="G31" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B32" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D32" t="s">
         <v>250</v>
@@ -13285,18 +13747,18 @@
         <v>250</v>
       </c>
       <c r="G32" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B33" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="H33" s="13" t="s">
         <v>275</v>
@@ -13304,10 +13766,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B34" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="E34" t="s">
         <v>250</v>
@@ -13316,259 +13778,259 @@
         <v>250</v>
       </c>
       <c r="G34" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B35" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D35" t="s">
         <v>250</v>
       </c>
       <c r="G35" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B36" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D36" t="s">
         <v>250</v>
       </c>
       <c r="G36" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B37" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B38" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B39" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="E39" t="s">
         <v>250</v>
       </c>
       <c r="G39" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B40" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="E40" t="s">
         <v>250</v>
       </c>
       <c r="G40" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B41" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="E41" t="s">
         <v>250</v>
       </c>
       <c r="G41" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B42" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="E42" t="s">
         <v>250</v>
       </c>
       <c r="G42" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B43" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B44" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B45" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B46" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B47" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B48" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B49" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B50" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B51" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="B52" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B53" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="B54" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B55" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B56" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B57" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B58" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B59" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B60" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B61" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
   </sheetData>
@@ -13826,36 +14288,36 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="102" t="s">
+        <v>564</v>
+      </c>
+      <c r="B1" s="102" t="s">
+        <v>565</v>
+      </c>
+      <c r="C1" s="103" t="s">
         <v>566</v>
       </c>
-      <c r="B1" s="102" t="s">
+      <c r="D1" s="102" t="s">
         <v>567</v>
       </c>
-      <c r="C1" s="103" t="s">
+      <c r="E1" s="102" t="s">
         <v>568</v>
-      </c>
-      <c r="D1" s="102" t="s">
-        <v>569</v>
-      </c>
-      <c r="E1" s="102" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
+        <v>569</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>570</v>
+      </c>
+      <c r="C2" s="65" t="s">
+        <v>570</v>
+      </c>
+      <c r="D2" s="65" t="s">
+        <v>570</v>
+      </c>
+      <c r="E2" s="65" t="s">
         <v>571</v>
-      </c>
-      <c r="B2" s="65" t="s">
-        <v>572</v>
-      </c>
-      <c r="C2" s="65" t="s">
-        <v>572</v>
-      </c>
-      <c r="D2" s="65" t="s">
-        <v>572</v>
-      </c>
-      <c r="E2" s="65" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -13863,10 +14325,10 @@
         <v>488</v>
       </c>
       <c r="B3" s="104" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E3" s="105" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -13874,10 +14336,10 @@
         <v>489</v>
       </c>
       <c r="B4" s="104" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="E4" s="105" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
@@ -13885,16 +14347,16 @@
         <v>490</v>
       </c>
       <c r="B5" s="107" t="s">
+        <v>576</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>577</v>
+      </c>
+      <c r="D5" s="107" t="s">
+        <v>576</v>
+      </c>
+      <c r="E5" s="108" t="s">
         <v>578</v>
-      </c>
-      <c r="C5" s="41" t="s">
-        <v>579</v>
-      </c>
-      <c r="D5" s="107" t="s">
-        <v>578</v>
-      </c>
-      <c r="E5" s="108" t="s">
-        <v>580</v>
       </c>
     </row>
   </sheetData>
@@ -13917,15 +14379,15 @@
   <sheetData>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B4" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -13933,7 +14395,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B19">
         <v>20</v>
@@ -13941,7 +14403,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B20">
         <v>22</v>
@@ -13949,7 +14411,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -13957,7 +14419,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B22">
         <v>1</v>

</xml_diff>